<commit_message>
realizada análise até o filtro de casos considerados plausíveis
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia.xlsx
@@ -583,7 +583,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -599,7 +599,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <bgColor rgb="FFFF3300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3300"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -643,7 +649,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -673,6 +679,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -740,7 +750,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFC000"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF3300"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -764,26 +774,26 @@
   <dimension ref="A1:N60"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.4336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.0816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.469387755102"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1023" min="14" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1023" min="14" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1183,7 +1193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -1192,17 +1202,17 @@
       </c>
       <c r="C10" s="2" t="n">
         <f aca="false">IF(I10="Incerto",MAX(G10,J10-(ABS(F10*J10))),J10)</f>
-        <v>50000</v>
+        <v>25000</v>
       </c>
       <c r="D10" s="2" t="n">
         <f aca="false">IF(I10="Incerto",MIN(H10,J10+(ABS(F10*J10))),J10)</f>
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G10" s="0" t="n">
         <f aca="false">J10/2</f>
@@ -1212,8 +1222,8 @@
         <f aca="false">J10*2</f>
         <v>100000</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>17</v>
+      <c r="I10" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="J10" s="1" t="n">
         <v>50000</v>
@@ -1225,7 +1235,7 @@
       <c r="M10" s="0"/>
       <c r="N10" s="1" t="n">
         <f aca="false">C10=D10</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1271,7 +1281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -1280,7 +1290,7 @@
       </c>
       <c r="C12" s="2" t="n">
         <f aca="false">IF(I12="Incerto",MAX(G12,J12-(ABS(F12*J12))),J12)</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D12" s="2" t="n">
         <f aca="false">IF(I12="Incerto",MIN(H12,J12+(ABS(F12*J12))),J12)</f>
@@ -1293,7 +1303,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>3</v>
@@ -1301,7 +1311,7 @@
       <c r="I12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="7" t="n">
+      <c r="J12" s="8" t="n">
         <v>0.4</v>
       </c>
       <c r="K12" s="1" t="n">
@@ -1986,7 +1996,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="9" t="s">
         <v>78</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -3261,10 +3271,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="6.3469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3320,11 +3330,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>140</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -3369,11 +3379,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Planilha com ampliação de incertezas
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia.xlsx
@@ -774,26 +774,26 @@
   <dimension ref="A1:N60"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.1530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.0816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.75"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="49.5408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.1989795918367"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1023" min="14" style="1" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1023" min="14" style="1" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.83163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,20 +1021,21 @@
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">IF(I6="Incerto",MAX(G6,J6-(ABS(F6*J6))),J6)</f>
-        <v>0.1</v>
+        <v>0.0666666666666667</v>
       </c>
       <c r="D6" s="2" t="n">
         <f aca="false">IF(I6="Incerto",MIN(H6,J6+(ABS(F6*J6))),J6)</f>
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>0</v>
+        <f aca="false">1/15</f>
+        <v>0.0666666666666667</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>1</v>
@@ -1247,11 +1248,11 @@
       </c>
       <c r="C11" s="2" t="n">
         <f aca="false">IF(I11="Incerto",MAX(G11,J11-(ABS(F11*J11))),J11)</f>
-        <v>0.001</v>
+        <v>0.0005</v>
       </c>
       <c r="D11" s="2" t="n">
         <f aca="false">IF(I11="Incerto",MIN(H11,J11+(ABS(F11*J11))),J11)</f>
-        <v>0.001</v>
+        <v>0.0015</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>33</v>
@@ -1266,7 +1267,7 @@
         <v>0.5</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J11" s="1" t="n">
         <v>0.001</v>
@@ -1278,7 +1279,7 @@
       <c r="M11" s="0"/>
       <c r="N11" s="1" t="n">
         <f aca="false">C11=D11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1423,7 +1424,7 @@
       </c>
       <c r="D15" s="2" t="n">
         <f aca="false">IF(I15="Incerto",MIN(H15,J15+(ABS(F15*J15))),J15)</f>
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>23</v>
@@ -1438,7 +1439,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J15" s="1" t="n">
         <v>0.25</v>
@@ -1454,7 +1455,7 @@
       </c>
       <c r="N15" s="1" t="n">
         <f aca="false">C15=D15</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1509,11 +1510,11 @@
       </c>
       <c r="C17" s="2" t="n">
         <f aca="false">IF(I17="Incerto",MAX(G17,J17-(ABS(F17*J17))),J17)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D17" s="2" t="n">
         <f aca="false">IF(I17="Incerto",MIN(H17,J17+(ABS(F17*J17))),J17)</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>23</v>
@@ -1528,7 +1529,7 @@
         <v>3</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J17" s="1" t="n">
         <v>1</v>
@@ -1544,7 +1545,7 @@
       </c>
       <c r="N17" s="1" t="n">
         <f aca="false">C17=D17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1642,11 +1643,11 @@
       </c>
       <c r="C20" s="2" t="n">
         <f aca="false">IF(I20="Incerto",MAX(G20,J20-(ABS(F20*J20))),J20)</f>
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="D20" s="2" t="n">
         <f aca="false">IF(I20="Incerto",MIN(H20,J20+(ABS(F20*J20))),J20)</f>
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>20</v>
@@ -1661,7 +1662,7 @@
         <v>20</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J20" s="1" t="n">
         <v>-4</v>
@@ -1673,7 +1674,7 @@
       <c r="M20" s="0"/>
       <c r="N20" s="1" t="n">
         <f aca="false">C20=D20</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1685,11 +1686,11 @@
       </c>
       <c r="C21" s="2" t="n">
         <f aca="false">IF(I21="Incerto",MAX(G21,J21-(ABS(F21*J21))),J21)</f>
-        <v>-8</v>
+        <v>-12</v>
       </c>
       <c r="D21" s="2" t="n">
         <f aca="false">IF(I21="Incerto",MIN(H21,J21+(ABS(F21*J21))),J21)</f>
-        <v>-8</v>
+        <v>-4</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>20</v>
@@ -1704,7 +1705,7 @@
         <v>20</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J21" s="1" t="n">
         <v>-8</v>
@@ -1720,7 +1721,7 @@
       </c>
       <c r="N21" s="1" t="n">
         <f aca="false">C21=D21</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1820,11 +1821,11 @@
       </c>
       <c r="C24" s="2" t="n">
         <f aca="false">IF(I24="Incerto",MAX(G24,J24-(ABS(F24*J24))),J24)</f>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="D24" s="2" t="n">
         <f aca="false">IF(I24="Incerto",MIN(H24,J24+(ABS(F24*J24))),J24)</f>
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>20</v>
@@ -1840,7 +1841,7 @@
         <v>9</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J24" s="1" t="n">
         <v>3</v>
@@ -1857,7 +1858,7 @@
       </c>
       <c r="N24" s="1" t="n">
         <f aca="false">C24=D24</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1914,11 +1915,11 @@
       </c>
       <c r="C26" s="2" t="n">
         <f aca="false">IF(I26="Incerto",MAX(G26,J26-(ABS(F26*J26))),J26)</f>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D26" s="2" t="n">
         <f aca="false">IF(I26="Incerto",MIN(H26,J26+(ABS(F26*J26))),J26)</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>33</v>
@@ -1933,7 +1934,7 @@
         <v>0.5</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J26" s="1" t="n">
         <v>0.2</v>
@@ -1945,7 +1946,7 @@
       <c r="M26" s="0"/>
       <c r="N26" s="1" t="n">
         <f aca="false">C26=D26</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1957,11 +1958,11 @@
       </c>
       <c r="C27" s="2" t="n">
         <f aca="false">IF(I27="Incerto",MAX(G27,J27-(ABS(F27*J27))),J27)</f>
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="D27" s="2" t="n">
         <f aca="false">IF(I27="Incerto",MIN(H27,J27+(ABS(F27*J27))),J27)</f>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>33</v>
@@ -1970,13 +1971,13 @@
         <v>0.5</v>
       </c>
       <c r="G27" s="1" t="n">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="H27" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J27" s="1" t="n">
         <v>0.8</v>
@@ -1992,7 +1993,7 @@
       </c>
       <c r="N27" s="1" t="n">
         <f aca="false">C27=D27</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2049,11 +2050,11 @@
       </c>
       <c r="C29" s="2" t="n">
         <f aca="false">IF(I29="Incerto",MAX(G29,J29-(ABS(F29*J29))),J29)</f>
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="D29" s="2" t="n">
         <f aca="false">IF(I29="Incerto",MIN(H29,J29+(ABS(F29*J29))),J29)</f>
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>33</v>
@@ -2062,13 +2063,13 @@
         <v>0.5</v>
       </c>
       <c r="G29" s="3" t="n">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="H29" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J29" s="1" t="n">
         <v>0.7</v>
@@ -2084,10 +2085,10 @@
       </c>
       <c r="N29" s="1" t="n">
         <f aca="false">C29=D29</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>83</v>
       </c>
@@ -2096,7 +2097,7 @@
       </c>
       <c r="C30" s="2" t="n">
         <f aca="false">IF(I30="Incerto",MAX(G30,J30-(ABS(F30*J30))),J30)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D30" s="2" t="n">
         <f aca="false">IF(I30="Incerto",MIN(H30,J30+(ABS(F30*J30))),J30)</f>
@@ -2113,7 +2114,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J30" s="1" t="n">
         <v>1</v>
@@ -2125,7 +2126,7 @@
       <c r="M30" s="0"/>
       <c r="N30" s="1" t="n">
         <f aca="false">C30=D30</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2264,11 +2265,11 @@
       </c>
       <c r="C34" s="2" t="n">
         <f aca="false">IF(I34="Incerto",MAX(G34,J34-(ABS(F34*J34))),J34)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D34" s="2" t="n">
         <f aca="false">IF(I34="Incerto",MIN(H34,J34+(ABS(F34*J34))),J34)</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>20</v>
@@ -2284,7 +2285,7 @@
         <v>3</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J34" s="1" t="n">
         <v>1</v>
@@ -2300,7 +2301,7 @@
       </c>
       <c r="N34" s="1" t="n">
         <f aca="false">C34=D34</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2312,11 +2313,11 @@
       </c>
       <c r="C35" s="2" t="n">
         <f aca="false">IF(I35="Incerto",MAX(G35,J35-(ABS(F35*J35))),J35)</f>
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D35" s="2" t="n">
         <f aca="false">IF(I35="Incerto",MIN(H35,J35+(ABS(F35*J35))),J35)</f>
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>20</v>
@@ -2332,7 +2333,7 @@
         <v>0.75</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J35" s="1" t="n">
         <v>0.25</v>
@@ -2348,7 +2349,7 @@
       </c>
       <c r="N35" s="1" t="n">
         <f aca="false">C35=D35</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2360,11 +2361,11 @@
       </c>
       <c r="C36" s="2" t="n">
         <f aca="false">IF(I36="Incerto",MAX(G36,J36-(ABS(F36*J36))),J36)</f>
-        <v>-0.1</v>
+        <v>-0.15</v>
       </c>
       <c r="D36" s="2" t="n">
         <f aca="false">IF(I36="Incerto",MIN(H36,J36+(ABS(F36*J36))),J36)</f>
-        <v>-0.1</v>
+        <v>-0.05</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>20</v>
@@ -2379,7 +2380,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J36" s="1" t="n">
         <v>-0.1</v>
@@ -2395,7 +2396,7 @@
       </c>
       <c r="N36" s="1" t="n">
         <f aca="false">C36=D36</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2522,11 +2523,11 @@
       </c>
       <c r="C40" s="2" t="n">
         <f aca="false">IF(I40="Incerto",MAX(G40,J40-(ABS(F40*J40))),J40)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D40" s="2" t="n">
         <f aca="false">IF(I40="Incerto",MIN(H40,J40+(ABS(F40*J40))),J40)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>23</v>
@@ -2542,7 +2543,7 @@
         <v>8</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J40" s="1" t="n">
         <v>4</v>
@@ -2599,11 +2600,11 @@
       </c>
       <c r="C42" s="2" t="n">
         <f aca="false">IF(I42="Incerto",MAX(G42,J42-(ABS(F42*J42))),J42)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" s="2" t="n">
         <f aca="false">IF(I42="Incerto",MIN(H42,J42+(ABS(F42*J42))),J42)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>23</v>
@@ -2620,7 +2621,7 @@
         <v>8</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J42" s="1" t="n">
         <v>2</v>
@@ -2638,11 +2639,11 @@
       </c>
       <c r="C43" s="2" t="n">
         <f aca="false">IF(I43="Incerto",MAX(G43,J43-(ABS(F43*J43))),J43)</f>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D43" s="2" t="n">
         <f aca="false">IF(I43="Incerto",MIN(H43,J43+(ABS(F43*J43))),J43)</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>102</v>
@@ -2658,7 +2659,7 @@
         <v>1</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J43" s="1" t="n">
         <v>0.4</v>
@@ -2715,11 +2716,11 @@
       </c>
       <c r="C45" s="2" t="n">
         <f aca="false">IF(I45="Incerto",MAX(G45,J45-(ABS(F45*J45))),J45)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D45" s="2" t="n">
         <f aca="false">IF(I45="Incerto",MIN(H45,J45+(ABS(F45*J45))),J45)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>23</v>
@@ -2736,7 +2737,7 @@
         <v>40</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J45" s="1" t="n">
         <v>10</v>
@@ -2754,11 +2755,11 @@
       </c>
       <c r="C46" s="2" t="n">
         <f aca="false">IF(I46="Incerto",MAX(G46,J46-(ABS(F46*J46))),J46)</f>
-        <v>0.0333333333333333</v>
+        <v>0.0166666666666667</v>
       </c>
       <c r="D46" s="2" t="n">
         <f aca="false">IF(I46="Incerto",MIN(H46,J46+(ABS(F46*J46))),J46)</f>
-        <v>0.0333333333333333</v>
+        <v>0.05</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>118</v>
@@ -2775,7 +2776,7 @@
         <v>0.133333333333333</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J46" s="1" t="n">
         <f aca="false">1/30</f>
@@ -2865,11 +2866,11 @@
       <c r="B49" s="0"/>
       <c r="C49" s="2" t="n">
         <f aca="false">IF(I49="Incerto",MAX(G49,J49-(ABS(F49*J49))),J49)</f>
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="D49" s="2" t="n">
         <f aca="false">IF(I49="Incerto",MIN(H49,J49+(ABS(F49*J49))),J49)</f>
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="F49" s="2" t="n">
         <v>0.5</v>
@@ -2881,7 +2882,7 @@
         <v>0</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="J49" s="1" t="n">
         <v>-4</v>
@@ -3271,10 +3272,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="6.20918367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3329,9 +3330,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
@@ -3379,11 +3377,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
rodando 16 estratégias, estratégia GBF ainda é robusta
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,10 @@
     <sheet name="configs" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="VariableNames" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$G$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$F$15</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -610,7 +614,7 @@
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -640,12 +644,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <u val="single"/>
@@ -722,7 +720,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -740,6 +738,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -767,15 +769,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -851,6 +845,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -858,27 +856,27 @@
   </sheetPr>
   <dimension ref="A1:N65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B91" activeCellId="0" sqref="B91"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F81" activeCellId="0" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="48.4642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="47.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.3877551020408"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.31632653061224"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.10204081632653"/>
     <col collapsed="false" hidden="false" max="1023" min="14" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.29081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -963,7 +961,7 @@
       </c>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
-      <c r="N2" s="1" t="n">
+      <c r="N2" s="5" t="n">
         <f aca="false">C2=D2</f>
         <v>1</v>
       </c>
@@ -1006,7 +1004,7 @@
       </c>
       <c r="L3" s="0"/>
       <c r="M3" s="0"/>
-      <c r="N3" s="1" t="n">
+      <c r="N3" s="5" t="n">
         <f aca="false">C3=D3</f>
         <v>1</v>
       </c>
@@ -1049,7 +1047,7 @@
       </c>
       <c r="L4" s="0"/>
       <c r="M4" s="0"/>
-      <c r="N4" s="1" t="n">
+      <c r="N4" s="5" t="n">
         <f aca="false">C4=D4</f>
         <v>1</v>
       </c>
@@ -1092,7 +1090,7 @@
       </c>
       <c r="L5" s="0"/>
       <c r="M5" s="0"/>
-      <c r="N5" s="1" t="n">
+      <c r="N5" s="5" t="n">
         <f aca="false">C5=D5</f>
         <v>1</v>
       </c>
@@ -1125,10 +1123,10 @@
       <c r="H6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="5" t="n">
+      <c r="J6" s="6" t="n">
         <f aca="false">1/5</f>
         <v>0.2</v>
       </c>
@@ -1141,7 +1139,7 @@
       <c r="M6" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="N6" s="1" t="n">
+      <c r="N6" s="5" t="n">
         <f aca="false">C6=D6</f>
         <v>0</v>
       </c>
@@ -1173,7 +1171,7 @@
       <c r="H7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="J7" s="1" t="n">
@@ -1184,7 +1182,7 @@
       </c>
       <c r="L7" s="0"/>
       <c r="M7" s="0"/>
-      <c r="N7" s="1" t="n">
+      <c r="N7" s="5" t="n">
         <f aca="false">C7=D7</f>
         <v>1</v>
       </c>
@@ -1227,7 +1225,7 @@
       </c>
       <c r="L8" s="0"/>
       <c r="M8" s="0"/>
-      <c r="N8" s="1" t="n">
+      <c r="N8" s="5" t="n">
         <f aca="false">C8=D8</f>
         <v>1</v>
       </c>
@@ -1259,7 +1257,7 @@
       <c r="H9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J9" s="1" t="n">
@@ -1274,7 +1272,7 @@
       <c r="M9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="N9" s="1" t="n">
+      <c r="N9" s="5" t="n">
         <f aca="false">C9=D9</f>
         <v>0</v>
       </c>
@@ -1308,7 +1306,7 @@
         <f aca="false">J10*2</f>
         <v>100000</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="8" t="s">
         <v>30</v>
       </c>
       <c r="J10" s="1" t="n">
@@ -1319,7 +1317,7 @@
       </c>
       <c r="L10" s="0"/>
       <c r="M10" s="0"/>
-      <c r="N10" s="1" t="n">
+      <c r="N10" s="5" t="n">
         <f aca="false">C10=D10</f>
         <v>0</v>
       </c>
@@ -1351,7 +1349,7 @@
       <c r="H11" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J11" s="1" t="n">
@@ -1362,7 +1360,7 @@
       </c>
       <c r="L11" s="0"/>
       <c r="M11" s="0"/>
-      <c r="N11" s="1" t="n">
+      <c r="N11" s="5" t="n">
         <f aca="false">C11=D11</f>
         <v>0</v>
       </c>
@@ -1394,10 +1392,10 @@
       <c r="H12" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="8" t="n">
+      <c r="J12" s="9" t="n">
         <v>0.4</v>
       </c>
       <c r="K12" s="1" t="n">
@@ -1405,7 +1403,7 @@
       </c>
       <c r="L12" s="0"/>
       <c r="M12" s="0"/>
-      <c r="N12" s="1" t="n">
+      <c r="N12" s="5" t="n">
         <f aca="false">C12=D12</f>
         <v>0</v>
       </c>
@@ -1439,10 +1437,10 @@
         <f aca="false">J13*10</f>
         <v>500000</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="5" t="n">
+      <c r="J13" s="6" t="n">
         <v>50000</v>
       </c>
       <c r="K13" s="1" t="n">
@@ -1450,7 +1448,7 @@
       </c>
       <c r="L13" s="0"/>
       <c r="M13" s="0"/>
-      <c r="N13" s="1" t="n">
+      <c r="N13" s="5" t="n">
         <f aca="false">C13=D13</f>
         <v>0</v>
       </c>
@@ -1491,7 +1489,7 @@
       </c>
       <c r="L14" s="0"/>
       <c r="M14" s="0"/>
-      <c r="N14" s="1" t="n">
+      <c r="N14" s="5" t="n">
         <f aca="false">C14=D14</f>
         <v>1</v>
       </c>
@@ -1523,7 +1521,7 @@
       <c r="H15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J15" s="1" t="n">
@@ -1538,7 +1536,7 @@
       <c r="M15" s="1" t="n">
         <v>0.25</v>
       </c>
-      <c r="N15" s="1" t="n">
+      <c r="N15" s="5" t="n">
         <f aca="false">C15=D15</f>
         <v>0</v>
       </c>
@@ -1581,7 +1579,7 @@
       </c>
       <c r="L16" s="0"/>
       <c r="M16" s="0"/>
-      <c r="N16" s="1" t="n">
+      <c r="N16" s="5" t="n">
         <f aca="false">C16=D16</f>
         <v>1</v>
       </c>
@@ -1613,7 +1611,7 @@
       <c r="H17" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J17" s="1" t="n">
@@ -1628,7 +1626,7 @@
       <c r="M17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N17" s="1" t="n">
+      <c r="N17" s="5" t="n">
         <f aca="false">C17=D17</f>
         <v>0</v>
       </c>
@@ -1671,7 +1669,7 @@
       </c>
       <c r="L18" s="0"/>
       <c r="M18" s="0"/>
-      <c r="N18" s="1" t="n">
+      <c r="N18" s="5" t="n">
         <f aca="false">C18=D18</f>
         <v>1</v>
       </c>
@@ -1714,7 +1712,7 @@
       </c>
       <c r="L19" s="0"/>
       <c r="M19" s="0"/>
-      <c r="N19" s="1" t="n">
+      <c r="N19" s="5" t="n">
         <f aca="false">C19=D19</f>
         <v>1</v>
       </c>
@@ -1746,7 +1744,7 @@
       <c r="H20" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J20" s="1" t="n">
@@ -1757,7 +1755,7 @@
       </c>
       <c r="L20" s="0"/>
       <c r="M20" s="0"/>
-      <c r="N20" s="1" t="n">
+      <c r="N20" s="5" t="n">
         <f aca="false">C20=D20</f>
         <v>0</v>
       </c>
@@ -1789,7 +1787,7 @@
       <c r="H21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J21" s="1" t="n">
@@ -1804,7 +1802,7 @@
       <c r="M21" s="1" t="n">
         <v>-4</v>
       </c>
-      <c r="N21" s="1" t="n">
+      <c r="N21" s="5" t="n">
         <f aca="false">C21=D21</f>
         <v>0</v>
       </c>
@@ -1836,7 +1834,7 @@
       <c r="H22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I22" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J22" s="1" t="n">
@@ -1847,7 +1845,7 @@
       </c>
       <c r="L22" s="0"/>
       <c r="M22" s="0"/>
-      <c r="N22" s="1" t="n">
+      <c r="N22" s="5" t="n">
         <f aca="false">C22=D22</f>
         <v>0</v>
       </c>
@@ -1892,7 +1890,7 @@
       </c>
       <c r="L23" s="0"/>
       <c r="M23" s="0"/>
-      <c r="N23" s="1" t="n">
+      <c r="N23" s="5" t="n">
         <f aca="false">C23=D23</f>
         <v>1</v>
       </c>
@@ -1925,7 +1923,7 @@
         <f aca="false">J24*3</f>
         <v>9</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J24" s="1" t="n">
@@ -1941,7 +1939,7 @@
       <c r="M24" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="N24" s="1" t="n">
+      <c r="N24" s="5" t="n">
         <f aca="false">C24=D24</f>
         <v>0</v>
       </c>
@@ -1973,7 +1971,7 @@
       <c r="H25" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="I25" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J25" s="1" t="n">
@@ -1984,7 +1982,7 @@
       </c>
       <c r="L25" s="0"/>
       <c r="M25" s="0"/>
-      <c r="N25" s="1" t="n">
+      <c r="N25" s="5" t="n">
         <f aca="false">C25=D25</f>
         <v>0</v>
       </c>
@@ -2016,7 +2014,7 @@
       <c r="H26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="I26" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J26" s="1" t="n">
@@ -2031,13 +2029,13 @@
       <c r="M26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N26" s="1" t="n">
+      <c r="N26" s="5" t="n">
         <f aca="false">C26=D26</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="10" t="s">
         <v>76</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2076,7 +2074,7 @@
       </c>
       <c r="L27" s="0"/>
       <c r="M27" s="0"/>
-      <c r="N27" s="1" t="n">
+      <c r="N27" s="5" t="n">
         <f aca="false">C27=D27</f>
         <v>1</v>
       </c>
@@ -2117,7 +2115,7 @@
       </c>
       <c r="L28" s="0"/>
       <c r="M28" s="0"/>
-      <c r="N28" s="1" t="n">
+      <c r="N28" s="5" t="n">
         <f aca="false">C28=D28</f>
         <v>1</v>
       </c>
@@ -2160,7 +2158,7 @@
       </c>
       <c r="L29" s="0"/>
       <c r="M29" s="0"/>
-      <c r="N29" s="1" t="n">
+      <c r="N29" s="5" t="n">
         <f aca="false">C29=D29</f>
         <v>1</v>
       </c>
@@ -2203,7 +2201,7 @@
       </c>
       <c r="L30" s="0"/>
       <c r="M30" s="0"/>
-      <c r="N30" s="1" t="n">
+      <c r="N30" s="5" t="n">
         <f aca="false">C30=D30</f>
         <v>1</v>
       </c>
@@ -2236,7 +2234,7 @@
         <f aca="false">J31*3</f>
         <v>3</v>
       </c>
-      <c r="I31" s="5" t="s">
+      <c r="I31" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J31" s="1" t="n">
@@ -2251,7 +2249,7 @@
       <c r="M31" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="N31" s="1" t="n">
+      <c r="N31" s="5" t="n">
         <f aca="false">C31=D31</f>
         <v>0</v>
       </c>
@@ -2284,7 +2282,7 @@
         <f aca="false">J32*3</f>
         <v>0.75</v>
       </c>
-      <c r="I32" s="5" t="s">
+      <c r="I32" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J32" s="1" t="n">
@@ -2299,7 +2297,7 @@
       <c r="M32" s="1" t="n">
         <v>0.25</v>
       </c>
-      <c r="N32" s="1" t="n">
+      <c r="N32" s="5" t="n">
         <f aca="false">C32=D32</f>
         <v>0</v>
       </c>
@@ -2331,7 +2329,7 @@
       <c r="H33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I33" s="5" t="s">
+      <c r="I33" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J33" s="1" t="n">
@@ -2346,7 +2344,7 @@
       <c r="M33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N33" s="1" t="n">
+      <c r="N33" s="5" t="n">
         <f aca="false">C33=D33</f>
         <v>0</v>
       </c>
@@ -2387,7 +2385,9 @@
       <c r="K34" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="N34" s="1" t="n">
+      <c r="L34" s="0"/>
+      <c r="M34" s="0"/>
+      <c r="N34" s="5" t="n">
         <f aca="false">C34=D34</f>
         <v>1</v>
       </c>
@@ -2401,11 +2401,11 @@
       </c>
       <c r="C35" s="2" t="n">
         <f aca="false">IF(I35="Incerto",MAX(G35,J35-(ABS(F35*J35))),J35)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="2" t="n">
         <f aca="false">IF(I35="Incerto",MIN(H35,J35+(ABS(F35*J35))),J35)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>20</v>
@@ -2423,11 +2423,14 @@
         <v>17</v>
       </c>
       <c r="J35" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="L35" s="0"/>
+      <c r="M35" s="0"/>
+      <c r="N35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
@@ -2457,7 +2460,7 @@
         <f aca="false">J36*2</f>
         <v>8</v>
       </c>
-      <c r="I36" s="5" t="s">
+      <c r="I36" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J36" s="1" t="n">
@@ -2466,6 +2469,9 @@
       <c r="K36" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="L36" s="0"/>
+      <c r="M36" s="0"/>
+      <c r="N36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
@@ -2496,7 +2502,7 @@
         <f aca="false">J37*4</f>
         <v>400000</v>
       </c>
-      <c r="I37" s="5" t="s">
+      <c r="I37" s="6" t="s">
         <v>17</v>
       </c>
       <c r="J37" s="1" t="n">
@@ -2505,6 +2511,9 @@
       <c r="K37" s="1" t="n">
         <v>100000</v>
       </c>
+      <c r="L37" s="0"/>
+      <c r="M37" s="0"/>
+      <c r="N37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
@@ -2535,7 +2544,7 @@
         <f aca="false">J38*4</f>
         <v>8</v>
       </c>
-      <c r="I38" s="5" t="s">
+      <c r="I38" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J38" s="1" t="n">
@@ -2544,6 +2553,9 @@
       <c r="K38" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="L38" s="0"/>
+      <c r="M38" s="0"/>
+      <c r="N38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
@@ -2573,7 +2585,7 @@
       <c r="H39" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I39" s="5" t="s">
+      <c r="I39" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J39" s="1" t="n">
@@ -2582,6 +2594,9 @@
       <c r="K39" s="1" t="n">
         <v>0.4</v>
       </c>
+      <c r="L39" s="0"/>
+      <c r="M39" s="0"/>
+      <c r="N39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
@@ -2621,6 +2636,9 @@
       <c r="K40" s="1" t="n">
         <v>18</v>
       </c>
+      <c r="L40" s="0"/>
+      <c r="M40" s="0"/>
+      <c r="N40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
@@ -2651,7 +2669,7 @@
         <f aca="false">J41*4</f>
         <v>40</v>
       </c>
-      <c r="I41" s="5" t="s">
+      <c r="I41" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J41" s="1" t="n">
@@ -2660,6 +2678,9 @@
       <c r="K41" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="L41" s="0"/>
+      <c r="M41" s="0"/>
+      <c r="N41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
@@ -2690,7 +2711,7 @@
         <f aca="false">J42*4</f>
         <v>0.133333333333333</v>
       </c>
-      <c r="I42" s="5" t="s">
+      <c r="I42" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J42" s="1" t="n">
@@ -2701,6 +2722,9 @@
         <f aca="false">1/30</f>
         <v>0.0333333333333333</v>
       </c>
+      <c r="L42" s="0"/>
+      <c r="M42" s="0"/>
+      <c r="N42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
@@ -2717,6 +2741,7 @@
         <f aca="false">IF(I43="Incerto",MIN(H43,J43+(ABS(F43*J43))),J43)</f>
         <v>0</v>
       </c>
+      <c r="E43" s="0"/>
       <c r="F43" s="2" t="n">
         <v>0.5</v>
       </c>
@@ -2737,6 +2762,9 @@
       <c r="K43" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="L43" s="0"/>
+      <c r="M43" s="0"/>
+      <c r="N43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
@@ -2753,6 +2781,7 @@
         <f aca="false">IF(I44="Incerto",MIN(H44,J44+(ABS(F44*J44))),J44)</f>
         <v>10</v>
       </c>
+      <c r="E44" s="0"/>
       <c r="F44" s="2" t="n">
         <v>0.5</v>
       </c>
@@ -2773,6 +2802,9 @@
       <c r="K44" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="L44" s="0"/>
+      <c r="M44" s="0"/>
+      <c r="N44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
@@ -2787,6 +2819,7 @@
         <f aca="false">IF(I45="Incerto",MIN(H45,J45+(ABS(F45*J45))),J45)</f>
         <v>-2</v>
       </c>
+      <c r="E45" s="0"/>
       <c r="F45" s="2" t="n">
         <v>0.5</v>
       </c>
@@ -2796,7 +2829,7 @@
       <c r="H45" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I45" s="5" t="s">
+      <c r="I45" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J45" s="1" t="n">
@@ -2805,6 +2838,9 @@
       <c r="K45" s="1" t="n">
         <v>-4</v>
       </c>
+      <c r="L45" s="0"/>
+      <c r="M45" s="0"/>
+      <c r="N45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
@@ -2819,6 +2855,7 @@
         <f aca="false">IF(I46="Incerto",MIN(H46,J46+(ABS(F46*J46))),J46)</f>
         <v>10</v>
       </c>
+      <c r="E46" s="0"/>
       <c r="F46" s="2" t="n">
         <v>0.5</v>
       </c>
@@ -2839,6 +2876,9 @@
       <c r="K46" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="L46" s="0"/>
+      <c r="M46" s="0"/>
+      <c r="N46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
@@ -2853,6 +2893,7 @@
         <f aca="false">IF(I47="Incerto",MIN(H47,J47+(ABS(F47*J47))),J47)</f>
         <v>2000</v>
       </c>
+      <c r="E47" s="0"/>
       <c r="F47" s="2" t="n">
         <v>0.5</v>
       </c>
@@ -2864,7 +2905,7 @@
         <f aca="false">J47*4</f>
         <v>8000</v>
       </c>
-      <c r="I47" s="5" t="s">
+      <c r="I47" s="6" t="s">
         <v>17</v>
       </c>
       <c r="J47" s="1" t="n">
@@ -2873,6 +2914,9 @@
       <c r="K47" s="1" t="n">
         <v>1000</v>
       </c>
+      <c r="L47" s="0"/>
+      <c r="M47" s="0"/>
+      <c r="N47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
@@ -2887,6 +2931,7 @@
         <f aca="false">IF(I48="Incerto",MIN(H48,J48+(ABS(F48*J48))),J48)</f>
         <v>200</v>
       </c>
+      <c r="E48" s="0"/>
       <c r="F48" s="2" t="n">
         <v>0.5</v>
       </c>
@@ -2898,7 +2943,7 @@
         <f aca="false">J48*4</f>
         <v>800</v>
       </c>
-      <c r="I48" s="5" t="s">
+      <c r="I48" s="6" t="s">
         <v>17</v>
       </c>
       <c r="J48" s="1" t="n">
@@ -2907,6 +2952,9 @@
       <c r="K48" s="1" t="n">
         <v>100</v>
       </c>
+      <c r="L48" s="0"/>
+      <c r="M48" s="0"/>
+      <c r="N48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
@@ -2921,6 +2969,7 @@
         <f aca="false">IF(I49="Incerto",MIN(H49,J49+(ABS(F49*J49))),J49)</f>
         <v>200</v>
       </c>
+      <c r="E49" s="0"/>
       <c r="F49" s="2" t="n">
         <v>0.5</v>
       </c>
@@ -2932,7 +2981,7 @@
         <f aca="false">J49*4</f>
         <v>800</v>
       </c>
-      <c r="I49" s="5" t="s">
+      <c r="I49" s="6" t="s">
         <v>17</v>
       </c>
       <c r="J49" s="1" t="n">
@@ -2941,6 +2990,9 @@
       <c r="K49" s="1" t="n">
         <v>100</v>
       </c>
+      <c r="L49" s="0"/>
+      <c r="M49" s="0"/>
+      <c r="N49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
@@ -2955,6 +3007,7 @@
         <f aca="false">IF(I50="Incerto",MIN(H50,J50+(ABS(F50*J50))),J50)</f>
         <v>20</v>
       </c>
+      <c r="E50" s="0"/>
       <c r="F50" s="2" t="n">
         <v>0.5</v>
       </c>
@@ -2966,7 +3019,7 @@
         <f aca="false">J50*4</f>
         <v>80</v>
       </c>
-      <c r="I50" s="5" t="s">
+      <c r="I50" s="6" t="s">
         <v>17</v>
       </c>
       <c r="J50" s="1" t="n">
@@ -2975,6 +3028,9 @@
       <c r="K50" s="1" t="n">
         <v>20</v>
       </c>
+      <c r="L50" s="0"/>
+      <c r="M50" s="0"/>
+      <c r="N50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
@@ -2989,6 +3045,7 @@
         <f aca="false">IF(I51="Incerto",MIN(H51,J51+(ABS(F51*J51))),J51)</f>
         <v>1000000</v>
       </c>
+      <c r="E51" s="0"/>
       <c r="F51" s="2" t="n">
         <v>0.5</v>
       </c>
@@ -3000,7 +3057,7 @@
         <f aca="false">J51*4</f>
         <v>4000000</v>
       </c>
-      <c r="I51" s="5" t="s">
+      <c r="I51" s="6" t="s">
         <v>17</v>
       </c>
       <c r="J51" s="1" t="n">
@@ -3009,11 +3066,15 @@
       <c r="K51" s="1" t="n">
         <v>1000000</v>
       </c>
+      <c r="L51" s="0"/>
+      <c r="M51" s="0"/>
+      <c r="N51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
         <v>122</v>
       </c>
+      <c r="B52" s="0"/>
       <c r="C52" s="2" t="n">
         <f aca="false">IF(I52="Incerto",MAX(G52,J52-(ABS(F52*J52))),J52)</f>
         <v>0.03</v>
@@ -3022,6 +3083,7 @@
         <f aca="false">IF(I52="Incerto",MIN(H52,J52+(ABS(F52*J52))),J52)</f>
         <v>0.9</v>
       </c>
+      <c r="E52" s="0"/>
       <c r="F52" s="2" t="n">
         <v>3</v>
       </c>
@@ -3037,11 +3099,16 @@
       <c r="J52" s="1" t="n">
         <v>0.4</v>
       </c>
+      <c r="K52" s="0"/>
+      <c r="L52" s="0"/>
+      <c r="M52" s="0"/>
+      <c r="N52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
         <v>123</v>
       </c>
+      <c r="B53" s="0"/>
       <c r="C53" s="2" t="n">
         <f aca="false">IF(I53="Incerto",MAX(G53,J53-(ABS(F53*J53))),J53)</f>
         <v>2500</v>
@@ -3050,6 +3117,7 @@
         <f aca="false">IF(I53="Incerto",MIN(H53,J53+(ABS(F53*J53))),J53)</f>
         <v>2500</v>
       </c>
+      <c r="E53" s="0"/>
       <c r="F53" s="2" t="n">
         <v>0.5</v>
       </c>
@@ -3067,11 +3135,16 @@
       <c r="J53" s="1" t="n">
         <v>2500</v>
       </c>
+      <c r="K53" s="0"/>
+      <c r="L53" s="0"/>
+      <c r="M53" s="0"/>
+      <c r="N53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="B54" s="0"/>
       <c r="C54" s="2" t="n">
         <f aca="false">IF(I54="Incerto",MAX(G54,J54-(ABS(F54*J54))),J54)</f>
         <v>1831</v>
@@ -3080,6 +3153,7 @@
         <f aca="false">IF(I54="Incerto",MIN(H54,J54+(ABS(F54*J54))),J54)</f>
         <v>1831</v>
       </c>
+      <c r="E54" s="0"/>
       <c r="F54" s="2" t="n">
         <v>0.5</v>
       </c>
@@ -3097,11 +3171,16 @@
       <c r="J54" s="1" t="n">
         <v>1831</v>
       </c>
+      <c r="K54" s="0"/>
+      <c r="L54" s="0"/>
+      <c r="M54" s="0"/>
+      <c r="N54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="B55" s="0"/>
       <c r="C55" s="2" t="n">
         <f aca="false">IF(I55="Incerto",MAX(G55,J55-(ABS(F55*J55))),J55)</f>
         <v>0.3</v>
@@ -3128,11 +3207,16 @@
       <c r="J55" s="1" t="n">
         <v>0.3</v>
       </c>
+      <c r="K55" s="0"/>
+      <c r="L55" s="0"/>
+      <c r="M55" s="0"/>
+      <c r="N55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="B56" s="0"/>
       <c r="C56" s="2" t="n">
         <f aca="false">IF(I56="Incerto",MAX(G56,J56-(ABS(F56*J56))),J56)</f>
         <v>0.3</v>
@@ -3159,11 +3243,16 @@
       <c r="J56" s="1" t="n">
         <v>0.3</v>
       </c>
+      <c r="K56" s="0"/>
+      <c r="L56" s="0"/>
+      <c r="M56" s="0"/>
+      <c r="N56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="B57" s="0"/>
       <c r="C57" s="2" t="n">
         <f aca="false">IF(I57="Incerto",MAX(G57,J57-(ABS(F57*J57))),J57)</f>
         <v>0.1</v>
@@ -3190,11 +3279,16 @@
       <c r="J57" s="1" t="n">
         <v>0.1</v>
       </c>
+      <c r="K57" s="0"/>
+      <c r="L57" s="0"/>
+      <c r="M57" s="0"/>
+      <c r="N57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
         <v>128</v>
       </c>
+      <c r="B58" s="0"/>
       <c r="C58" s="2" t="n">
         <f aca="false">IF(I58="Incerto",MAX(G58,J58-(ABS(F58*J58))),J58)</f>
         <v>0.3</v>
@@ -3221,6 +3315,10 @@
       <c r="J58" s="1" t="n">
         <v>0.3</v>
       </c>
+      <c r="K58" s="0"/>
+      <c r="L58" s="0"/>
+      <c r="M58" s="0"/>
+      <c r="N58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
@@ -3259,11 +3357,15 @@
       <c r="K59" s="1" t="n">
         <v>0.5</v>
       </c>
+      <c r="L59" s="0"/>
+      <c r="M59" s="0"/>
+      <c r="N59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="B60" s="0"/>
       <c r="C60" s="2" t="n">
         <f aca="false">IF(I60="Incerto",MAX(G60,J60-(ABS(F60*J60))),J60)</f>
         <v>0.3</v>
@@ -3291,11 +3393,16 @@
         <f aca="false">J56</f>
         <v>0.3</v>
       </c>
+      <c r="K60" s="0"/>
+      <c r="L60" s="0"/>
+      <c r="M60" s="0"/>
+      <c r="N60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
         <v>132</v>
       </c>
+      <c r="B61" s="0"/>
       <c r="C61" s="2" t="n">
         <f aca="false">IF(I61="Incerto",MAX(G61,J61-(ABS(F61*J61))),J61)</f>
         <v>0.1</v>
@@ -3323,11 +3430,16 @@
         <f aca="false">J57</f>
         <v>0.1</v>
       </c>
+      <c r="K61" s="0"/>
+      <c r="L61" s="0"/>
+      <c r="M61" s="0"/>
+      <c r="N61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="B62" s="0"/>
       <c r="C62" s="2" t="n">
         <f aca="false">IF(I62="Incerto",MAX(G62,J62-(ABS(F62*J62))),J62)</f>
         <v>0.3</v>
@@ -3355,6 +3467,10 @@
         <f aca="false">J58</f>
         <v>0.3</v>
       </c>
+      <c r="K62" s="0"/>
+      <c r="L62" s="0"/>
+      <c r="M62" s="0"/>
+      <c r="N62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
@@ -3389,6 +3505,10 @@
       <c r="J63" s="1" t="n">
         <v>0.5</v>
       </c>
+      <c r="K63" s="0"/>
+      <c r="L63" s="0"/>
+      <c r="M63" s="0"/>
+      <c r="N63" s="0"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
@@ -3423,6 +3543,10 @@
       <c r="J64" s="1" t="n">
         <v>0.5</v>
       </c>
+      <c r="K64" s="0"/>
+      <c r="L64" s="0"/>
+      <c r="M64" s="0"/>
+      <c r="N64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
@@ -3457,6 +3581,10 @@
       <c r="J65" s="1" t="n">
         <v>0.5</v>
       </c>
+      <c r="K65" s="0"/>
+      <c r="L65" s="0"/>
+      <c r="M65" s="0"/>
+      <c r="N65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
@@ -3465,11 +3593,11 @@
       <c r="B66" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C66" s="10" t="n">
+      <c r="C66" s="11" t="n">
         <f aca="false">IF(I66="Incerto",MAX(G66,J66-(ABS(F66*J66))),J66)</f>
         <v>0.001</v>
       </c>
-      <c r="D66" s="10" t="n">
+      <c r="D66" s="11" t="n">
         <f aca="false">IF(I66="Incerto",MIN(H66,J66+(ABS(F66*J66))),J66)</f>
         <v>0.005</v>
       </c>
@@ -3485,7 +3613,7 @@
       <c r="H66" s="1" t="n">
         <v>0.005</v>
       </c>
-      <c r="I66" s="5" t="s">
+      <c r="I66" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J66" s="1" t="n">
@@ -3494,6 +3622,9 @@
       <c r="K66" s="1" t="n">
         <v>0.001</v>
       </c>
+      <c r="L66" s="0"/>
+      <c r="M66" s="0"/>
+      <c r="N66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
@@ -3502,11 +3633,11 @@
       <c r="B67" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C67" s="10" t="n">
+      <c r="C67" s="11" t="n">
         <f aca="false">IF(I67="Incerto",MAX(G67,J67-(ABS(F67*J67))),J67)</f>
         <v>0.001</v>
       </c>
-      <c r="D67" s="10" t="n">
+      <c r="D67" s="11" t="n">
         <f aca="false">IF(I67="Incerto",MIN(H67,J67+(ABS(F67*J67))),J67)</f>
         <v>0.005</v>
       </c>
@@ -3522,7 +3653,7 @@
       <c r="H67" s="1" t="n">
         <v>0.005</v>
       </c>
-      <c r="I67" s="5" t="s">
+      <c r="I67" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J67" s="1" t="n">
@@ -3531,6 +3662,9 @@
       <c r="K67" s="1" t="n">
         <v>0.001</v>
       </c>
+      <c r="L67" s="0"/>
+      <c r="M67" s="0"/>
+      <c r="N67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
@@ -3539,11 +3673,11 @@
       <c r="B68" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C68" s="10" t="n">
+      <c r="C68" s="11" t="n">
         <f aca="false">IF(I68="Incerto",MAX(G68,J68-(ABS(F68*J68))),J68)</f>
         <v>0.001</v>
       </c>
-      <c r="D68" s="10" t="n">
+      <c r="D68" s="11" t="n">
         <f aca="false">IF(I68="Incerto",MIN(H68,J68+(ABS(F68*J68))),J68)</f>
         <v>0.005</v>
       </c>
@@ -3559,7 +3693,7 @@
       <c r="H68" s="1" t="n">
         <v>0.005</v>
       </c>
-      <c r="I68" s="5" t="s">
+      <c r="I68" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J68" s="1" t="n">
@@ -3568,6 +3702,9 @@
       <c r="K68" s="1" t="n">
         <v>0.001</v>
       </c>
+      <c r="L68" s="0"/>
+      <c r="M68" s="0"/>
+      <c r="N68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
@@ -3596,23 +3733,23 @@
       <c r="H69" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I69" s="5" t="s">
+      <c r="I69" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J69" s="1" t="n">
         <f aca="false">J56</f>
         <v>0.3</v>
       </c>
-      <c r="K69" s="5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L69" s="5" t="n">
+      <c r="K69" s="6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L69" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="M69" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="N69" s="11" t="n">
+      <c r="M69" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N69" s="5" t="n">
         <f aca="false">C69=D69</f>
         <v>0</v>
       </c>
@@ -3644,23 +3781,23 @@
       <c r="H70" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I70" s="5" t="s">
+      <c r="I70" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J70" s="1" t="n">
         <f aca="false">J57</f>
         <v>0.1</v>
       </c>
-      <c r="K70" s="5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L70" s="5" t="n">
+      <c r="K70" s="6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L70" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="M70" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="N70" s="11" t="n">
+      <c r="M70" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N70" s="5" t="n">
         <f aca="false">C70=D70</f>
         <v>0</v>
       </c>
@@ -3692,23 +3829,23 @@
       <c r="H71" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I71" s="5" t="s">
+      <c r="I71" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J71" s="1" t="n">
         <f aca="false">J58</f>
         <v>0.3</v>
       </c>
-      <c r="K71" s="5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L71" s="5" t="n">
+      <c r="K71" s="6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L71" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="M71" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="N71" s="11" t="n">
+      <c r="M71" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N71" s="5" t="n">
         <f aca="false">C71=D71</f>
         <v>0</v>
       </c>
@@ -3738,7 +3875,7 @@
       <c r="H72" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I72" s="5" t="s">
+      <c r="I72" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J72" s="1" t="n">
@@ -3749,7 +3886,7 @@
       </c>
       <c r="L72" s="0"/>
       <c r="M72" s="0"/>
-      <c r="N72" s="11" t="n">
+      <c r="N72" s="5" t="n">
         <f aca="false">C72=D72</f>
         <v>0</v>
       </c>
@@ -3779,7 +3916,7 @@
       <c r="H73" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I73" s="5" t="s">
+      <c r="I73" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J73" s="1" t="n">
@@ -3790,7 +3927,7 @@
       </c>
       <c r="L73" s="0"/>
       <c r="M73" s="0"/>
-      <c r="N73" s="11" t="n">
+      <c r="N73" s="5" t="n">
         <f aca="false">C73=D73</f>
         <v>0</v>
       </c>
@@ -3820,7 +3957,7 @@
       <c r="H74" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I74" s="5" t="s">
+      <c r="I74" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J74" s="1" t="n">
@@ -3831,7 +3968,7 @@
       </c>
       <c r="L74" s="0"/>
       <c r="M74" s="0"/>
-      <c r="N74" s="11" t="n">
+      <c r="N74" s="5" t="n">
         <f aca="false">C74=D74</f>
         <v>0</v>
       </c>
@@ -3876,7 +4013,7 @@
       </c>
       <c r="L75" s="0"/>
       <c r="M75" s="0"/>
-      <c r="N75" s="11" t="n">
+      <c r="N75" s="5" t="n">
         <f aca="false">C75=D75</f>
         <v>1</v>
       </c>
@@ -3921,7 +4058,7 @@
       </c>
       <c r="L76" s="0"/>
       <c r="M76" s="0"/>
-      <c r="N76" s="11" t="n">
+      <c r="N76" s="5" t="n">
         <f aca="false">C76=D76</f>
         <v>1</v>
       </c>
@@ -3966,7 +4103,7 @@
       </c>
       <c r="L77" s="0"/>
       <c r="M77" s="0"/>
-      <c r="N77" s="11" t="n">
+      <c r="N77" s="5" t="n">
         <f aca="false">C77=D77</f>
         <v>1</v>
       </c>
@@ -4011,7 +4148,7 @@
       </c>
       <c r="L78" s="0"/>
       <c r="M78" s="0"/>
-      <c r="N78" s="11" t="n">
+      <c r="N78" s="5" t="n">
         <f aca="false">C78=D78</f>
         <v>1</v>
       </c>
@@ -4036,20 +4173,20 @@
   </sheetPr>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.8571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.0357142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.0714285714286"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -4069,10 +4206,10 @@
       <c r="E1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="1" t="s">
         <v>161</v>
       </c>
       <c r="H1" s="0"/>
@@ -4477,6 +4614,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G17"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4484,6 +4622,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4500,11 +4639,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>162</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -4549,11 +4688,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
estratégias dos players mais agressiva
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia.xlsx
@@ -5,20 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="levers" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="configs" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="VariableNames" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Levers_FullDesign" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Levers_FullDesign" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="levers" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="configs" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="VariableNames" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -497,6 +498,18 @@
     <t xml:space="preserve">aInitialPrice4</t>
   </si>
   <si>
+    <t xml:space="preserve">aSwitchForCapacityStrategy1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aPercPeDAberto1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aDesiredMarketShare1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aOrcamentoPeD1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lever</t>
   </si>
   <si>
@@ -504,18 +517,6 @@
   </si>
   <si>
     <t xml:space="preserve">CasoBase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aSwitchForCapacityStrategy1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aPercPeDAberto1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aDesiredMarketShare1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aOrcamentoPeD1</t>
   </si>
   <si>
     <t xml:space="preserve">Start</t>
@@ -855,27 +856,27 @@
   </sheetPr>
   <dimension ref="A1:N65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B70" activeCellId="0" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="45.4897959183674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.8469387755102"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.77551020408163"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="7.69387755102041"/>
     <col collapsed="false" hidden="false" max="1023" min="14" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.88265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3182,11 +3183,11 @@
       <c r="B55" s="0"/>
       <c r="C55" s="2" t="n">
         <f aca="false">IF(I55="Incerto",MAX(G55,J55-(ABS(F55*J55))),J55)</f>
-        <v>0.3</v>
+        <v>0.28</v>
       </c>
       <c r="D55" s="2" t="n">
         <f aca="false">IF(I55="Incerto",MIN(H55,J55+(ABS(F55*J55))),J55)</f>
-        <v>0.3</v>
+        <v>0.28</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>103</v>
@@ -3204,7 +3205,7 @@
         <v>17</v>
       </c>
       <c r="J55" s="1" t="n">
-        <v>0.3</v>
+        <v>0.28</v>
       </c>
       <c r="K55" s="0"/>
       <c r="L55" s="0"/>
@@ -3218,11 +3219,11 @@
       <c r="B56" s="0"/>
       <c r="C56" s="2" t="n">
         <f aca="false">IF(I56="Incerto",MAX(G56,J56-(ABS(F56*J56))),J56)</f>
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D56" s="2" t="n">
         <f aca="false">IF(I56="Incerto",MIN(H56,J56+(ABS(F56*J56))),J56)</f>
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>103</v>
@@ -3240,7 +3241,7 @@
         <v>17</v>
       </c>
       <c r="J56" s="1" t="n">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="K56" s="0"/>
       <c r="L56" s="0"/>
@@ -3254,11 +3255,11 @@
       <c r="B57" s="0"/>
       <c r="C57" s="2" t="n">
         <f aca="false">IF(I57="Incerto",MAX(G57,J57-(ABS(F57*J57))),J57)</f>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="D57" s="2" t="n">
         <f aca="false">IF(I57="Incerto",MIN(H57,J57+(ABS(F57*J57))),J57)</f>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>103</v>
@@ -3276,7 +3277,7 @@
         <v>17</v>
       </c>
       <c r="J57" s="1" t="n">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="K57" s="0"/>
       <c r="L57" s="0"/>
@@ -3290,11 +3291,11 @@
       <c r="B58" s="0"/>
       <c r="C58" s="2" t="n">
         <f aca="false">IF(I58="Incerto",MAX(G58,J58-(ABS(F58*J58))),J58)</f>
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
       <c r="D58" s="2" t="n">
         <f aca="false">IF(I58="Incerto",MIN(H58,J58+(ABS(F58*J58))),J58)</f>
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>103</v>
@@ -3312,7 +3313,8 @@
         <v>17</v>
       </c>
       <c r="J58" s="1" t="n">
-        <v>0.3</v>
+        <f aca="false">1-SUM(J55:J57)</f>
+        <v>0.32</v>
       </c>
       <c r="K58" s="0"/>
       <c r="L58" s="0"/>
@@ -3328,11 +3330,11 @@
       </c>
       <c r="C59" s="2" t="n">
         <f aca="false">IF(I59="Incerto",MAX(G59,J59-(ABS(F59*J59))),J59)</f>
-        <v>0.3</v>
+        <v>0.28</v>
       </c>
       <c r="D59" s="2" t="n">
         <f aca="false">IF(I59="Incerto",MIN(H59,J59+(ABS(F59*J59))),J59)</f>
-        <v>0.3</v>
+        <v>0.28</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>103</v>
@@ -3351,7 +3353,7 @@
       </c>
       <c r="J59" s="1" t="n">
         <f aca="false">J55</f>
-        <v>0.3</v>
+        <v>0.28</v>
       </c>
       <c r="K59" s="1" t="n">
         <v>0.5</v>
@@ -3367,11 +3369,11 @@
       <c r="B60" s="0"/>
       <c r="C60" s="2" t="n">
         <f aca="false">IF(I60="Incerto",MAX(G60,J60-(ABS(F60*J60))),J60)</f>
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D60" s="2" t="n">
         <f aca="false">IF(I60="Incerto",MIN(H60,J60+(ABS(F60*J60))),J60)</f>
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>103</v>
@@ -3390,7 +3392,7 @@
       </c>
       <c r="J60" s="1" t="n">
         <f aca="false">J56</f>
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="K60" s="0"/>
       <c r="L60" s="0"/>
@@ -3404,11 +3406,11 @@
       <c r="B61" s="0"/>
       <c r="C61" s="2" t="n">
         <f aca="false">IF(I61="Incerto",MAX(G61,J61-(ABS(F61*J61))),J61)</f>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="D61" s="2" t="n">
         <f aca="false">IF(I61="Incerto",MIN(H61,J61+(ABS(F61*J61))),J61)</f>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>103</v>
@@ -3427,7 +3429,7 @@
       </c>
       <c r="J61" s="1" t="n">
         <f aca="false">J57</f>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="K61" s="0"/>
       <c r="L61" s="0"/>
@@ -3441,11 +3443,11 @@
       <c r="B62" s="0"/>
       <c r="C62" s="2" t="n">
         <f aca="false">IF(I62="Incerto",MAX(G62,J62-(ABS(F62*J62))),J62)</f>
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
       <c r="D62" s="2" t="n">
         <f aca="false">IF(I62="Incerto",MIN(H62,J62+(ABS(F62*J62))),J62)</f>
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>103</v>
@@ -3464,7 +3466,7 @@
       </c>
       <c r="J62" s="1" t="n">
         <f aca="false">J58</f>
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
       <c r="K62" s="0"/>
       <c r="L62" s="0"/>
@@ -3714,11 +3716,11 @@
       </c>
       <c r="C69" s="2" t="n">
         <f aca="false">IF(I69="Incerto",MAX(G69,J69-(ABS(F69*J69))),J69)</f>
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="D69" s="2" t="n">
         <f aca="false">IF(I69="Incerto",MIN(H69,J69+(ABS(F69*J69))),J69)</f>
-        <v>0.45</v>
+        <v>0.375</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>33</v>
@@ -3727,7 +3729,8 @@
         <v>0.5</v>
       </c>
       <c r="G69" s="1" t="n">
-        <v>0.2</v>
+        <f aca="false">J56</f>
+        <v>0.25</v>
       </c>
       <c r="H69" s="1" t="n">
         <v>1</v>
@@ -3737,7 +3740,7 @@
       </c>
       <c r="J69" s="1" t="n">
         <f aca="false">J56</f>
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="K69" s="5" t="n">
         <v>0.5</v>
@@ -3762,11 +3765,11 @@
       </c>
       <c r="C70" s="2" t="n">
         <f aca="false">IF(I70="Incerto",MAX(G70,J70-(ABS(F70*J70))),J70)</f>
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="D70" s="2" t="n">
         <f aca="false">IF(I70="Incerto",MIN(H70,J70+(ABS(F70*J70))),J70)</f>
-        <v>0.15</v>
+        <v>0.225</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>33</v>
@@ -3775,7 +3778,8 @@
         <v>0.5</v>
       </c>
       <c r="G70" s="1" t="n">
-        <v>0.05</v>
+        <f aca="false">J57</f>
+        <v>0.15</v>
       </c>
       <c r="H70" s="1" t="n">
         <v>1</v>
@@ -3785,7 +3789,7 @@
       </c>
       <c r="J70" s="1" t="n">
         <f aca="false">J57</f>
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="K70" s="5" t="n">
         <v>0.5</v>
@@ -3810,11 +3814,11 @@
       </c>
       <c r="C71" s="2" t="n">
         <f aca="false">IF(I71="Incerto",MAX(G71,J71-(ABS(F71*J71))),J71)</f>
-        <v>0.2</v>
+        <v>0.32</v>
       </c>
       <c r="D71" s="2" t="n">
         <f aca="false">IF(I71="Incerto",MIN(H71,J71+(ABS(F71*J71))),J71)</f>
-        <v>0.45</v>
+        <v>0.48</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>33</v>
@@ -3823,7 +3827,8 @@
         <v>0.5</v>
       </c>
       <c r="G71" s="1" t="n">
-        <v>0.2</v>
+        <f aca="false">J58</f>
+        <v>0.32</v>
       </c>
       <c r="H71" s="1" t="n">
         <v>1</v>
@@ -3833,7 +3838,7 @@
       </c>
       <c r="J71" s="1" t="n">
         <f aca="false">J58</f>
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
       <c r="K71" s="5" t="n">
         <v>0.5</v>
@@ -4170,47 +4175,128 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.0714285714286"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.15</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.530612244898"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="I1" s="0"/>
     </row>
@@ -4253,7 +4339,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H17"/>
+  <autoFilter ref="A1:G15"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4265,7 +4351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4278,7 +4364,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4301,175 +4387,6 @@
       </c>
       <c r="C2" s="0" t="n">
         <v>0.125</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E12"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
-        <v>184</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -4488,78 +4405,166 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0.3</v>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tornando as estratégias dos outros players agressiva
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia.xlsx
@@ -15,11 +15,12 @@
     <sheet name="VariableNames" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -857,26 +858,26 @@
   <dimension ref="A1:N65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B70" activeCellId="0" sqref="B70"/>
+      <selection pane="topLeft" activeCell="I75" activeCellId="0" sqref="I75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="45.4897959183674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.5816326530612"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.50510204081633"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="7.56122448979592"/>
     <col collapsed="false" hidden="false" max="1023" min="14" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3596,11 +3597,11 @@
       </c>
       <c r="C66" s="10" t="n">
         <f aca="false">IF(I66="Incerto",MAX(G66,J66-(ABS(F66*J66))),J66)</f>
-        <v>0.001</v>
+        <v>0.05</v>
       </c>
       <c r="D66" s="10" t="n">
         <f aca="false">IF(I66="Incerto",MIN(H66,J66+(ABS(F66*J66))),J66)</f>
-        <v>0.005</v>
+        <v>0.006</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>103</v>
@@ -3609,10 +3610,12 @@
         <v>5</v>
       </c>
       <c r="G66" s="1" t="n">
-        <v>0.001</v>
+        <f aca="false">MIN(Levers_FullDesign!$D$2:$D$12)</f>
+        <v>0.05</v>
       </c>
       <c r="H66" s="1" t="n">
-        <v>0.005</v>
+        <f aca="false">MAX(Levers_FullDesign!$D$2:$D$14)</f>
+        <v>0.1</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>30</v>
@@ -3636,11 +3639,11 @@
       </c>
       <c r="C67" s="10" t="n">
         <f aca="false">IF(I67="Incerto",MAX(G67,J67-(ABS(F67*J67))),J67)</f>
-        <v>0.001</v>
+        <v>0.05</v>
       </c>
       <c r="D67" s="10" t="n">
         <f aca="false">IF(I67="Incerto",MIN(H67,J67+(ABS(F67*J67))),J67)</f>
-        <v>0.005</v>
+        <v>0.006</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>103</v>
@@ -3649,10 +3652,12 @@
         <v>5</v>
       </c>
       <c r="G67" s="1" t="n">
-        <v>0.001</v>
+        <f aca="false">MIN(Levers_FullDesign!$D$2:$D$12)</f>
+        <v>0.05</v>
       </c>
       <c r="H67" s="1" t="n">
-        <v>0.005</v>
+        <f aca="false">MAX(Levers_FullDesign!$D$2:$D$14)</f>
+        <v>0.1</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>30</v>
@@ -3676,11 +3681,11 @@
       </c>
       <c r="C68" s="10" t="n">
         <f aca="false">IF(I68="Incerto",MAX(G68,J68-(ABS(F68*J68))),J68)</f>
-        <v>0.001</v>
+        <v>0.05</v>
       </c>
       <c r="D68" s="10" t="n">
         <f aca="false">IF(I68="Incerto",MIN(H68,J68+(ABS(F68*J68))),J68)</f>
-        <v>0.005</v>
+        <v>0.006</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>103</v>
@@ -3689,10 +3694,12 @@
         <v>5</v>
       </c>
       <c r="G68" s="1" t="n">
-        <v>0.001</v>
+        <f aca="false">MIN(Levers_FullDesign!$D$2:$D$12)</f>
+        <v>0.05</v>
       </c>
       <c r="H68" s="1" t="n">
-        <v>0.005</v>
+        <f aca="false">MAX(Levers_FullDesign!$D$2:$D$14)</f>
+        <v>0.1</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>30</v>
@@ -3863,7 +3870,7 @@
       </c>
       <c r="C72" s="2" t="n">
         <f aca="false">IF(I72="Incerto",MAX(G72,J72-(ABS(F72*J72))),J72)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D72" s="2" t="n">
         <f aca="false">IF(I72="Incerto",MIN(H72,J72+(ABS(F72*J72))),J72)</f>
@@ -3880,7 +3887,7 @@
         <v>1</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="J72" s="1" t="n">
         <v>1</v>
@@ -3892,7 +3899,7 @@
       <c r="M72" s="0"/>
       <c r="N72" s="1" t="n">
         <f aca="false">C72=D72</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3904,7 +3911,7 @@
       </c>
       <c r="C73" s="2" t="n">
         <f aca="false">IF(I73="Incerto",MAX(G73,J73-(ABS(F73*J73))),J73)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D73" s="2" t="n">
         <f aca="false">IF(I73="Incerto",MIN(H73,J73+(ABS(F73*J73))),J73)</f>
@@ -3921,7 +3928,7 @@
         <v>1</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="J73" s="1" t="n">
         <v>1</v>
@@ -3933,7 +3940,7 @@
       <c r="M73" s="0"/>
       <c r="N73" s="1" t="n">
         <f aca="false">C73=D73</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3945,7 +3952,7 @@
       </c>
       <c r="C74" s="2" t="n">
         <f aca="false">IF(I74="Incerto",MAX(G74,J74-(ABS(F74*J74))),J74)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74" s="2" t="n">
         <f aca="false">IF(I74="Incerto",MIN(H74,J74+(ABS(F74*J74))),J74)</f>
@@ -3962,7 +3969,7 @@
         <v>1</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="J74" s="1" t="n">
         <v>1</v>
@@ -3974,7 +3981,7 @@
       <c r="M74" s="0"/>
       <c r="N74" s="1" t="n">
         <f aca="false">C74=D74</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4175,19 +4182,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4220,24 +4227,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="n">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.28</v>
+        <v>0.45</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0.15</v>
       </c>
     </row>
   </sheetData>
@@ -4265,14 +4261,14 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.3928571428571"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -4339,7 +4335,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G15"/>
+  <autoFilter ref="A1:H17"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4364,7 +4360,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4413,11 +4409,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
modelo está melhor calibrado agora.
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia.xlsx
@@ -16,11 +16,14 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$G$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="193">
   <si>
     <t xml:space="preserve">Variavel</t>
   </si>
@@ -74,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Igual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inc</t>
   </si>
   <si>
     <t xml:space="preserve">aUnitsPerHousehold</t>
@@ -725,7 +731,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -743,6 +749,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -850,34 +860,40 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N65536"/>
+  <dimension ref="A1:O65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I75" activeCellId="0" sqref="I75"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="44.8163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.0408163265306"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.23469387755102"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.530612244898"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="1023" min="14" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="17.6479591836735"/>
+    <col collapsed="false" hidden="false" max="1023" min="16" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.47959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -923,13 +939,16 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="n">
         <f aca="false">IF(I2="Incerto",MAX(G2,J2-(ABS(F2*J2))),J2)</f>
@@ -940,7 +959,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0.5</v>
@@ -952,7 +971,7 @@
         <v>30</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>1</v>
@@ -966,13 +985,17 @@
         <f aca="false">C2=D2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O2" s="5" t="n">
+        <f aca="false">D2&gt;C2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2" t="n">
         <f aca="false">IF(I3="Incerto",MAX(G3,J3-(ABS(F3*J3))),J3)</f>
@@ -983,7 +1006,7 @@
         <v>0.04</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0.5</v>
@@ -995,7 +1018,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0.04</v>
@@ -1009,13 +1032,17 @@
         <f aca="false">C3=D3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O3" s="5" t="n">
+        <f aca="false">D3&gt;C3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="n">
         <f aca="false">IF(I4="Incerto",MAX(G4,J4-(ABS(F4*J4))),J4)</f>
@@ -1026,7 +1053,7 @@
         <v>0.25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="n">
         <v>0.5</v>
@@ -1038,7 +1065,7 @@
         <v>10</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>0.25</v>
@@ -1052,13 +1079,17 @@
         <f aca="false">C4=D4</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O4" s="5" t="n">
+        <f aca="false">D4&gt;C4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="n">
         <f aca="false">IF(I5="Incerto",MAX(G5,J5-(ABS(F5*J5))),J5)</f>
@@ -1069,7 +1100,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0.5</v>
@@ -1081,7 +1112,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J5" s="1" t="n">
         <v>1</v>
@@ -1095,13 +1126,17 @@
         <f aca="false">C5=D5</f>
         <v>1</v>
       </c>
+      <c r="O5" s="5" t="n">
+        <f aca="false">D5&gt;C5</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="n">
         <f aca="false">IF(I6="Incerto",MAX(G6,J6-(ABS(F6*J6))),J6)</f>
@@ -1112,7 +1147,7 @@
         <v>0.6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>2</v>
@@ -1124,10 +1159,10 @@
       <c r="H6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="5" t="n">
+      <c r="I6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="6" t="n">
         <f aca="false">1/5</f>
         <v>0.2</v>
       </c>
@@ -1144,13 +1179,17 @@
         <f aca="false">C6=D6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O6" s="5" t="n">
+        <f aca="false">D6&gt;C6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="n">
         <f aca="false">IF(I7="Incerto",MAX(G7,J7-(ABS(F7*J7))),J7)</f>
@@ -1161,7 +1200,7 @@
         <v>0.05</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F7" s="2" t="n">
         <v>0.5</v>
@@ -1172,8 +1211,8 @@
       <c r="H7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>17</v>
+      <c r="I7" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="J7" s="1" t="n">
         <v>0.05</v>
@@ -1187,13 +1226,17 @@
         <f aca="false">C7=D7</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O7" s="5" t="n">
+        <f aca="false">D7&gt;C7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2" t="n">
         <f aca="false">IF(I8="Incerto",MAX(G8,J8-(ABS(F8*J8))),J8)</f>
@@ -1204,7 +1247,7 @@
         <v>200000</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F8" s="2" t="n">
         <v>0.5</v>
@@ -1216,7 +1259,7 @@
         <v>200000</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J8" s="1" t="n">
         <v>200000</v>
@@ -1230,13 +1273,17 @@
         <f aca="false">C8=D8</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O8" s="5" t="n">
+        <f aca="false">D8&gt;C8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2" t="n">
         <f aca="false">IF(I9="Incerto",MAX(G9,J9-(ABS(F9*J9))),J9)</f>
@@ -1247,7 +1294,7 @@
         <v>0.3</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F9" s="2" t="n">
         <v>0.5</v>
@@ -1258,8 +1305,8 @@
       <c r="H9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>30</v>
+      <c r="I9" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J9" s="1" t="n">
         <v>0.2</v>
@@ -1277,13 +1324,17 @@
         <f aca="false">C9=D9</f>
         <v>0</v>
       </c>
+      <c r="O9" s="5" t="n">
+        <f aca="false">D9&gt;C9</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2" t="n">
         <f aca="false">IF(I10="Incerto",MAX(G10,J10-(ABS(F10*J10))),J10)</f>
@@ -1294,7 +1345,7 @@
         <v>100000</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F10" s="2" t="n">
         <v>1</v>
@@ -1307,8 +1358,8 @@
         <f aca="false">J10*2</f>
         <v>100000</v>
       </c>
-      <c r="I10" s="7" t="s">
-        <v>30</v>
+      <c r="I10" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="J10" s="1" t="n">
         <v>50000</v>
@@ -1322,13 +1373,17 @@
         <f aca="false">C10=D10</f>
         <v>0</v>
       </c>
+      <c r="O10" s="5" t="n">
+        <f aca="false">D10&gt;C10</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" s="2" t="n">
         <f aca="false">IF(I11="Incerto",MAX(G11,J11-(ABS(F11*J11))),J11)</f>
@@ -1339,7 +1394,7 @@
         <v>0.0015</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F11" s="2" t="n">
         <v>0.5</v>
@@ -1350,8 +1405,8 @@
       <c r="H11" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>30</v>
+      <c r="I11" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J11" s="1" t="n">
         <v>0.001</v>
@@ -1365,13 +1420,17 @@
         <f aca="false">C11=D11</f>
         <v>0</v>
       </c>
+      <c r="O11" s="5" t="n">
+        <f aca="false">D11&gt;C11</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2" t="n">
         <f aca="false">IF(I12="Incerto",MAX(G12,J12-(ABS(F12*J12))),J12)</f>
@@ -1382,7 +1441,7 @@
         <v>1.6</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>3</v>
@@ -1393,10 +1452,10 @@
       <c r="H12" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="8" t="n">
+      <c r="I12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="9" t="n">
         <v>0.4</v>
       </c>
       <c r="K12" s="1" t="n">
@@ -1408,13 +1467,17 @@
         <f aca="false">C12=D12</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O12" s="5" t="n">
+        <f aca="false">D12&gt;C12</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C13" s="2" t="n">
         <f aca="false">IF(I13="Incerto",MAX(G13,J13-(ABS(F13*J13))),J13)</f>
@@ -1425,7 +1488,7 @@
         <v>300000</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F13" s="2" t="n">
         <v>5</v>
@@ -1438,10 +1501,10 @@
         <f aca="false">J13*10</f>
         <v>500000</v>
       </c>
-      <c r="I13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J13" s="5" t="n">
+      <c r="I13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="6" t="n">
         <v>50000</v>
       </c>
       <c r="K13" s="1" t="n">
@@ -1453,13 +1516,17 @@
         <f aca="false">C13=D13</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O13" s="5" t="n">
+        <f aca="false">D13&gt;C13</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" s="2" t="n">
         <f aca="false">IF(I14="Incerto",MAX(G14,J14-(ABS(F14*J14))),J14)</f>
@@ -1480,7 +1547,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J14" s="1" t="n">
         <v>0</v>
@@ -1494,13 +1561,17 @@
         <f aca="false">C14=D14</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O14" s="5" t="n">
+        <f aca="false">D14&gt;C14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C15" s="2" t="n">
         <f aca="false">IF(I15="Incerto",MAX(G15,J15-(ABS(F15*J15))),J15)</f>
@@ -1511,7 +1582,7 @@
         <v>0.375</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>0.5</v>
@@ -1522,8 +1593,8 @@
       <c r="H15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>30</v>
+      <c r="I15" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J15" s="1" t="n">
         <v>0.25</v>
@@ -1541,13 +1612,17 @@
         <f aca="false">C15=D15</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O15" s="5" t="n">
+        <f aca="false">D15&gt;C15</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C16" s="2" t="n">
         <f aca="false">IF(I16="Incerto",MAX(G16,J16-(ABS(F16*J16))),J16)</f>
@@ -1558,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>0.5</v>
@@ -1570,7 +1645,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J16" s="1" t="n">
         <v>1</v>
@@ -1584,13 +1659,17 @@
         <f aca="false">C16=D16</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O16" s="5" t="n">
+        <f aca="false">D16&gt;C16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C17" s="2" t="n">
         <f aca="false">IF(I17="Incerto",MAX(G17,J17-(ABS(F17*J17))),J17)</f>
@@ -1601,7 +1680,7 @@
         <v>1.5</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>0.5</v>
@@ -1612,8 +1691,8 @@
       <c r="H17" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>30</v>
+      <c r="I17" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J17" s="1" t="n">
         <v>1</v>
@@ -1631,13 +1710,17 @@
         <f aca="false">C17=D17</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O17" s="5" t="n">
+        <f aca="false">D17&gt;C17</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C18" s="2" t="n">
         <f aca="false">IF(I18="Incerto",MAX(G18,J18-(ABS(F18*J18))),J18)</f>
@@ -1648,7 +1731,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>0.5</v>
@@ -1660,7 +1743,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J18" s="1" t="n">
         <v>1</v>
@@ -1674,13 +1757,17 @@
         <f aca="false">C18=D18</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O18" s="5" t="n">
+        <f aca="false">D18&gt;C18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C19" s="2" t="n">
         <f aca="false">IF(I19="Incerto",MAX(G19,J19-(ABS(F19*J19))),J19)</f>
@@ -1691,7 +1778,7 @@
         <v>0.25</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>0.5</v>
@@ -1703,7 +1790,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J19" s="1" t="n">
         <v>0.25</v>
@@ -1717,13 +1804,17 @@
         <f aca="false">C19=D19</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O19" s="5" t="n">
+        <f aca="false">D19&gt;C19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C20" s="2" t="n">
         <f aca="false">IF(I20="Incerto",MAX(G20,J20-(ABS(F20*J20))),J20)</f>
@@ -1734,7 +1825,7 @@
         <v>-2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0.5</v>
@@ -1745,8 +1836,8 @@
       <c r="H20" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>30</v>
+      <c r="I20" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J20" s="1" t="n">
         <v>-4</v>
@@ -1760,13 +1851,17 @@
         <f aca="false">C20=D20</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O20" s="5" t="n">
+        <f aca="false">D20&gt;C20</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C21" s="2" t="n">
         <f aca="false">IF(I21="Incerto",MAX(G21,J21-(ABS(F21*J21))),J21)</f>
@@ -1777,7 +1872,7 @@
         <v>-4</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F21" s="2" t="n">
         <v>0.5</v>
@@ -1788,8 +1883,8 @@
       <c r="H21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="I21" s="5" t="s">
-        <v>30</v>
+      <c r="I21" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J21" s="1" t="n">
         <v>-8</v>
@@ -1807,13 +1902,17 @@
         <f aca="false">C21=D21</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O21" s="5" t="n">
+        <f aca="false">D21&gt;C21</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C22" s="2" t="n">
         <f aca="false">IF(I22="Incerto",MAX(G22,J22-(ABS(F22*J22))),J22)</f>
@@ -1824,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F22" s="2" t="n">
         <v>0.5</v>
@@ -1835,8 +1934,8 @@
       <c r="H22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I22" s="5" t="s">
-        <v>30</v>
+      <c r="I22" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J22" s="1" t="n">
         <v>0.7</v>
@@ -1850,13 +1949,17 @@
         <f aca="false">C22=D22</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O22" s="5" t="n">
+        <f aca="false">D22&gt;C22</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C23" s="2" t="n">
         <f aca="false">IF(H23="Incerto",MAX(G23,J23-(ABS(F23*J23))),J23)</f>
@@ -1867,7 +1970,7 @@
         <v>100000</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F23" s="2" t="n">
         <v>0.5</v>
@@ -1881,7 +1984,7 @@
         <v>200000</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J23" s="1" t="n">
         <v>100000</v>
@@ -1895,13 +1998,17 @@
         <f aca="false">C23=D23</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O23" s="5" t="n">
+        <f aca="false">D23&gt;C23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C24" s="2" t="n">
         <f aca="false">IF(I24="Incerto",MAX(G24,J24-(ABS(F24*J24))),J24)</f>
@@ -1912,7 +2019,7 @@
         <v>4.5</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F24" s="2" t="n">
         <v>0.5</v>
@@ -1924,8 +2031,8 @@
         <f aca="false">J24*3</f>
         <v>9</v>
       </c>
-      <c r="I24" s="5" t="s">
-        <v>30</v>
+      <c r="I24" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J24" s="1" t="n">
         <v>3</v>
@@ -1944,13 +2051,17 @@
         <f aca="false">C24=D24</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O24" s="5" t="n">
+        <f aca="false">D24&gt;C24</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C25" s="2" t="n">
         <f aca="false">IF(I25="Incerto",MAX(G25,J25-(ABS(F25*J25))),J25)</f>
@@ -1961,7 +2072,7 @@
         <v>0.3</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F25" s="2" t="n">
         <v>0.5</v>
@@ -1972,8 +2083,8 @@
       <c r="H25" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>30</v>
+      <c r="I25" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J25" s="1" t="n">
         <v>0.2</v>
@@ -1987,13 +2098,17 @@
         <f aca="false">C25=D25</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O25" s="5" t="n">
+        <f aca="false">D25&gt;C25</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="2" t="n">
         <f aca="false">IF(I26="Incerto",MAX(G26,J26-(ABS(F26*J26))),J26)</f>
@@ -2004,7 +2119,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F26" s="2" t="n">
         <v>0.5</v>
@@ -2015,8 +2130,8 @@
       <c r="H26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I26" s="5" t="s">
-        <v>30</v>
+      <c r="I26" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J26" s="1" t="n">
         <v>0.8</v>
@@ -2034,13 +2149,17 @@
         <f aca="false">C26=D26</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="9" t="s">
-        <v>76</v>
+      <c r="O26" s="5" t="n">
+        <f aca="false">D26&gt;C26</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C27" s="2" t="n">
         <f aca="false">IF(I27="Incerto",MAX(G27,J27-(ABS(F27*J27))),J27)</f>
@@ -2051,7 +2170,7 @@
         <v>10</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F27" s="2" t="n">
         <v>0.5</v>
@@ -2065,7 +2184,7 @@
         <v>20</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J27" s="1" t="n">
         <v>10</v>
@@ -2079,13 +2198,17 @@
         <f aca="false">C27=D27</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O27" s="5" t="n">
+        <f aca="false">D27&gt;C27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C28" s="2" t="n">
         <f aca="false">IF(I28="Incerto",MAX(G28,J28-(ABS(F28*J28))),J28)</f>
@@ -2106,7 +2229,7 @@
         <v>1</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J28" s="1" t="n">
         <v>1</v>
@@ -2120,13 +2243,17 @@
         <f aca="false">C28=D28</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O28" s="5" t="n">
+        <f aca="false">D28&gt;C28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C29" s="2" t="n">
         <f aca="false">IF(I29="Incerto",MAX(G29,J29-(ABS(F29*J29))),J29)</f>
@@ -2137,7 +2264,7 @@
         <v>0.25</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F29" s="2" t="n">
         <v>0.5</v>
@@ -2149,7 +2276,7 @@
         <v>0.25</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J29" s="1" t="n">
         <v>0.25</v>
@@ -2163,13 +2290,17 @@
         <f aca="false">C29=D29</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O29" s="5" t="n">
+        <f aca="false">D29&gt;C29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C30" s="2" t="n">
         <f aca="false">IF(I30="Incerto",MAX(G30,J30-(ABS(F30*J30))),J30)</f>
@@ -2180,7 +2311,7 @@
         <v>0.25</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F30" s="2" t="n">
         <v>0.5</v>
@@ -2192,7 +2323,7 @@
         <v>0.25</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J30" s="1" t="n">
         <v>0.25</v>
@@ -2206,13 +2337,17 @@
         <f aca="false">C30=D30</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O30" s="5" t="n">
+        <f aca="false">D30&gt;C30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C31" s="2" t="n">
         <f aca="false">IF(I31="Incerto",MAX(G31,J31-(ABS(F31*J31))),J31)</f>
@@ -2223,7 +2358,7 @@
         <v>1.5</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F31" s="2" t="n">
         <v>0.5</v>
@@ -2235,8 +2370,8 @@
         <f aca="false">J31*3</f>
         <v>3</v>
       </c>
-      <c r="I31" s="5" t="s">
-        <v>30</v>
+      <c r="I31" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J31" s="1" t="n">
         <v>1</v>
@@ -2254,13 +2389,17 @@
         <f aca="false">C31=D31</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O31" s="5" t="n">
+        <f aca="false">D31&gt;C31</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C32" s="2" t="n">
         <f aca="false">IF(I32="Incerto",MAX(G32,J32-(ABS(F32*J32))),J32)</f>
@@ -2271,7 +2410,7 @@
         <v>0.375</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F32" s="2" t="n">
         <v>0.5</v>
@@ -2283,8 +2422,8 @@
         <f aca="false">J32*3</f>
         <v>0.75</v>
       </c>
-      <c r="I32" s="5" t="s">
-        <v>30</v>
+      <c r="I32" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J32" s="1" t="n">
         <v>0.25</v>
@@ -2302,13 +2441,17 @@
         <f aca="false">C32=D32</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O32" s="5" t="n">
+        <f aca="false">D32&gt;C32</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C33" s="2" t="n">
         <f aca="false">IF(I33="Incerto",MAX(G33,J33-(ABS(F33*J33))),J33)</f>
@@ -2319,7 +2462,7 @@
         <v>-0.05</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F33" s="2" t="n">
         <v>0.5</v>
@@ -2330,8 +2473,8 @@
       <c r="H33" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I33" s="5" t="s">
-        <v>30</v>
+      <c r="I33" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J33" s="1" t="n">
         <v>-0.1</v>
@@ -2349,13 +2492,17 @@
         <f aca="false">C33=D33</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O33" s="5" t="n">
+        <f aca="false">D33&gt;C33</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C34" s="2" t="n">
         <f aca="false">IF(I34="Incerto",MAX(G34,J34-(ABS(F34*J34))),J34)</f>
@@ -2366,7 +2513,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F34" s="2" t="n">
         <v>0.5</v>
@@ -2378,7 +2525,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J34" s="1" t="n">
         <v>0</v>
@@ -2392,13 +2539,17 @@
         <f aca="false">C34=D34</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O34" s="5" t="n">
+        <f aca="false">D34&gt;C34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C35" s="2" t="n">
         <f aca="false">IF(I35="Incerto",MAX(G35,J35-(ABS(F35*J35))),J35)</f>
@@ -2409,7 +2560,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F35" s="2" t="n">
         <v>0.5</v>
@@ -2421,7 +2572,7 @@
         <v>1</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J35" s="1" t="n">
         <v>1</v>
@@ -2432,13 +2583,17 @@
       <c r="L35" s="0"/>
       <c r="M35" s="0"/>
       <c r="N35" s="0"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O35" s="5" t="n">
+        <f aca="false">D35&gt;C35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C36" s="2" t="n">
         <f aca="false">IF(I36="Incerto",MAX(G36,J36-(ABS(F36*J36))),J36)</f>
@@ -2449,7 +2604,7 @@
         <v>6</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F36" s="2" t="n">
         <v>0.5</v>
@@ -2461,8 +2616,8 @@
         <f aca="false">J36*2</f>
         <v>8</v>
       </c>
-      <c r="I36" s="5" t="s">
-        <v>30</v>
+      <c r="I36" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J36" s="1" t="n">
         <v>4</v>
@@ -2473,13 +2628,17 @@
       <c r="L36" s="0"/>
       <c r="M36" s="0"/>
       <c r="N36" s="0"/>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O36" s="5" t="n">
+        <f aca="false">D36&gt;C36</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C37" s="2" t="n">
         <f aca="false">IF(I37="Incerto",MAX(G37,J37-(ABS(F37*J37))),J37)</f>
@@ -2490,7 +2649,7 @@
         <v>100000</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F37" s="2" t="n">
         <v>0.5</v>
@@ -2503,8 +2662,8 @@
         <f aca="false">J37*4</f>
         <v>400000</v>
       </c>
-      <c r="I37" s="5" t="s">
-        <v>17</v>
+      <c r="I37" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="J37" s="1" t="n">
         <v>100000</v>
@@ -2515,13 +2674,17 @@
       <c r="L37" s="0"/>
       <c r="M37" s="0"/>
       <c r="N37" s="0"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O37" s="5" t="n">
+        <f aca="false">D37&gt;C37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C38" s="2" t="n">
         <f aca="false">IF(I38="Incerto",MAX(G38,J38-(ABS(F38*J38))),J38)</f>
@@ -2532,7 +2695,7 @@
         <v>3</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F38" s="2" t="n">
         <v>0.5</v>
@@ -2545,8 +2708,8 @@
         <f aca="false">J38*4</f>
         <v>8</v>
       </c>
-      <c r="I38" s="5" t="s">
-        <v>30</v>
+      <c r="I38" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J38" s="1" t="n">
         <v>2</v>
@@ -2557,13 +2720,17 @@
       <c r="L38" s="0"/>
       <c r="M38" s="0"/>
       <c r="N38" s="0"/>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O38" s="5" t="n">
+        <f aca="false">D38&gt;C38</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C39" s="2" t="n">
         <f aca="false">IF(I39="Incerto",MAX(G39,J39-(ABS(F39*J39))),J39)</f>
@@ -2574,7 +2741,7 @@
         <v>0.6</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F39" s="2" t="n">
         <v>0.5</v>
@@ -2586,8 +2753,8 @@
       <c r="H39" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I39" s="5" t="s">
-        <v>30</v>
+      <c r="I39" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J39" s="1" t="n">
         <v>0.4</v>
@@ -2598,13 +2765,17 @@
       <c r="L39" s="0"/>
       <c r="M39" s="0"/>
       <c r="N39" s="0"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O39" s="5" t="n">
+        <f aca="false">D39&gt;C39</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C40" s="2" t="n">
         <f aca="false">IF(I40="Incerto",MAX(G40,J40-(ABS(F40*J40))),J40)</f>
@@ -2615,7 +2786,7 @@
         <v>18</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F40" s="2" t="n">
         <v>0.5</v>
@@ -2629,7 +2800,7 @@
         <v>72</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J40" s="1" t="n">
         <v>18</v>
@@ -2640,13 +2811,17 @@
       <c r="L40" s="0"/>
       <c r="M40" s="0"/>
       <c r="N40" s="0"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O40" s="5" t="n">
+        <f aca="false">D40&gt;C40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C41" s="2" t="n">
         <f aca="false">IF(I41="Incerto",MAX(G41,J41-(ABS(F41*J41))),J41)</f>
@@ -2657,7 +2832,7 @@
         <v>15</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F41" s="2" t="n">
         <v>0.5</v>
@@ -2670,8 +2845,8 @@
         <f aca="false">J41*4</f>
         <v>40</v>
       </c>
-      <c r="I41" s="5" t="s">
-        <v>30</v>
+      <c r="I41" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J41" s="1" t="n">
         <v>10</v>
@@ -2682,13 +2857,17 @@
       <c r="L41" s="0"/>
       <c r="M41" s="0"/>
       <c r="N41" s="0"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O41" s="5" t="n">
+        <f aca="false">D41&gt;C41</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C42" s="2" t="n">
         <f aca="false">IF(I42="Incerto",MAX(G42,J42-(ABS(F42*J42))),J42)</f>
@@ -2699,7 +2878,7 @@
         <v>0.05</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F42" s="2" t="n">
         <v>0.5</v>
@@ -2712,8 +2891,8 @@
         <f aca="false">J42*4</f>
         <v>0.133333333333333</v>
       </c>
-      <c r="I42" s="5" t="s">
-        <v>30</v>
+      <c r="I42" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J42" s="1" t="n">
         <f aca="false">1/30</f>
@@ -2726,13 +2905,17 @@
       <c r="L42" s="0"/>
       <c r="M42" s="0"/>
       <c r="N42" s="0"/>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O42" s="5" t="n">
+        <f aca="false">D42&gt;C42</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C43" s="2" t="n">
         <f aca="false">IF(I43="Incerto",MAX(G43,J43-(ABS(F43*J43))),J43)</f>
@@ -2755,7 +2938,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J43" s="1" t="n">
         <v>0</v>
@@ -2766,13 +2949,17 @@
       <c r="L43" s="0"/>
       <c r="M43" s="0"/>
       <c r="N43" s="0"/>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O43" s="5" t="n">
+        <f aca="false">D43&gt;C43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C44" s="2" t="n">
         <f aca="false">IF(I44="Incerto",MAX(G44,J44-(ABS(F44*J44))),J44)</f>
@@ -2795,7 +2982,7 @@
         <v>40</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J44" s="1" t="n">
         <v>10</v>
@@ -2806,10 +2993,14 @@
       <c r="L44" s="0"/>
       <c r="M44" s="0"/>
       <c r="N44" s="0"/>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O44" s="5" t="n">
+        <f aca="false">D44&gt;C44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B45" s="0"/>
       <c r="C45" s="2" t="n">
@@ -2830,8 +3021,8 @@
       <c r="H45" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I45" s="5" t="s">
-        <v>30</v>
+      <c r="I45" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J45" s="1" t="n">
         <v>-4</v>
@@ -2842,10 +3033,14 @@
       <c r="L45" s="0"/>
       <c r="M45" s="0"/>
       <c r="N45" s="0"/>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O45" s="5" t="n">
+        <f aca="false">D45&gt;C45</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B46" s="0"/>
       <c r="C46" s="2" t="n">
@@ -2869,7 +3064,7 @@
         <v>40</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J46" s="1" t="n">
         <v>10</v>
@@ -2880,10 +3075,14 @@
       <c r="L46" s="0"/>
       <c r="M46" s="0"/>
       <c r="N46" s="0"/>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O46" s="5" t="n">
+        <f aca="false">D46&gt;C46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="2" t="n">
@@ -2906,8 +3105,8 @@
         <f aca="false">J47*4</f>
         <v>8000</v>
       </c>
-      <c r="I47" s="5" t="s">
-        <v>17</v>
+      <c r="I47" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="J47" s="1" t="n">
         <v>2000</v>
@@ -2918,10 +3117,14 @@
       <c r="L47" s="0"/>
       <c r="M47" s="0"/>
       <c r="N47" s="0"/>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O47" s="5" t="n">
+        <f aca="false">D47&gt;C47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B48" s="0"/>
       <c r="C48" s="2" t="n">
@@ -2944,8 +3147,8 @@
         <f aca="false">J48*4</f>
         <v>800</v>
       </c>
-      <c r="I48" s="5" t="s">
-        <v>17</v>
+      <c r="I48" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="J48" s="1" t="n">
         <v>200</v>
@@ -2956,10 +3159,14 @@
       <c r="L48" s="0"/>
       <c r="M48" s="0"/>
       <c r="N48" s="0"/>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O48" s="5" t="n">
+        <f aca="false">D48&gt;C48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B49" s="0"/>
       <c r="C49" s="2" t="n">
@@ -2982,8 +3189,8 @@
         <f aca="false">J49*4</f>
         <v>800</v>
       </c>
-      <c r="I49" s="5" t="s">
-        <v>17</v>
+      <c r="I49" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="J49" s="1" t="n">
         <v>200</v>
@@ -2994,10 +3201,14 @@
       <c r="L49" s="0"/>
       <c r="M49" s="0"/>
       <c r="N49" s="0"/>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O49" s="5" t="n">
+        <f aca="false">D49&gt;C49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B50" s="0"/>
       <c r="C50" s="2" t="n">
@@ -3020,8 +3231,8 @@
         <f aca="false">J50*4</f>
         <v>80</v>
       </c>
-      <c r="I50" s="5" t="s">
-        <v>17</v>
+      <c r="I50" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="J50" s="1" t="n">
         <v>20</v>
@@ -3032,10 +3243,14 @@
       <c r="L50" s="0"/>
       <c r="M50" s="0"/>
       <c r="N50" s="0"/>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O50" s="5" t="n">
+        <f aca="false">D50&gt;C50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B51" s="0"/>
       <c r="C51" s="2" t="n">
@@ -3058,8 +3273,8 @@
         <f aca="false">J51*4</f>
         <v>4000000</v>
       </c>
-      <c r="I51" s="5" t="s">
-        <v>17</v>
+      <c r="I51" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="J51" s="1" t="n">
         <v>1000000</v>
@@ -3070,10 +3285,14 @@
       <c r="L51" s="0"/>
       <c r="M51" s="0"/>
       <c r="N51" s="0"/>
+      <c r="O51" s="5" t="n">
+        <f aca="false">D51&gt;C51</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B52" s="0"/>
       <c r="C52" s="2" t="n">
@@ -3095,7 +3314,7 @@
         <v>0.9</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J52" s="1" t="n">
         <v>0.4</v>
@@ -3104,10 +3323,14 @@
       <c r="L52" s="0"/>
       <c r="M52" s="0"/>
       <c r="N52" s="0"/>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O52" s="5" t="n">
+        <f aca="false">D52&gt;C52</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B53" s="0"/>
       <c r="C53" s="2" t="n">
@@ -3131,7 +3354,7 @@
         <v>25000</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J53" s="1" t="n">
         <v>2500</v>
@@ -3140,10 +3363,14 @@
       <c r="L53" s="0"/>
       <c r="M53" s="0"/>
       <c r="N53" s="0"/>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O53" s="5" t="n">
+        <f aca="false">D53&gt;C53</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B54" s="0"/>
       <c r="C54" s="2" t="n">
@@ -3167,7 +3394,7 @@
         <v>18310</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J54" s="1" t="n">
         <v>1831</v>
@@ -3176,10 +3403,14 @@
       <c r="L54" s="0"/>
       <c r="M54" s="0"/>
       <c r="N54" s="0"/>
+      <c r="O54" s="5" t="n">
+        <f aca="false">D54&gt;C54</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B55" s="0"/>
       <c r="C55" s="2" t="n">
@@ -3191,7 +3422,7 @@
         <v>0.28</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F55" s="2" t="n">
         <v>0.5</v>
@@ -3203,7 +3434,7 @@
         <v>1</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J55" s="1" t="n">
         <v>0.28</v>
@@ -3212,10 +3443,14 @@
       <c r="L55" s="0"/>
       <c r="M55" s="0"/>
       <c r="N55" s="0"/>
+      <c r="O55" s="5" t="n">
+        <f aca="false">D55&gt;C55</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B56" s="0"/>
       <c r="C56" s="2" t="n">
@@ -3227,7 +3462,7 @@
         <v>0.25</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F56" s="2" t="n">
         <v>0.5</v>
@@ -3239,7 +3474,7 @@
         <v>1</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J56" s="1" t="n">
         <v>0.25</v>
@@ -3248,10 +3483,14 @@
       <c r="L56" s="0"/>
       <c r="M56" s="0"/>
       <c r="N56" s="0"/>
+      <c r="O56" s="5" t="n">
+        <f aca="false">D56&gt;C56</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B57" s="0"/>
       <c r="C57" s="2" t="n">
@@ -3263,7 +3502,7 @@
         <v>0.15</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F57" s="2" t="n">
         <v>0.5</v>
@@ -3275,7 +3514,7 @@
         <v>1</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J57" s="1" t="n">
         <v>0.15</v>
@@ -3284,10 +3523,14 @@
       <c r="L57" s="0"/>
       <c r="M57" s="0"/>
       <c r="N57" s="0"/>
+      <c r="O57" s="5" t="n">
+        <f aca="false">D57&gt;C57</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B58" s="0"/>
       <c r="C58" s="2" t="n">
@@ -3299,7 +3542,7 @@
         <v>0.32</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F58" s="2" t="n">
         <v>0.5</v>
@@ -3311,7 +3554,7 @@
         <v>1</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J58" s="1" t="n">
         <f aca="false">1-SUM(J55:J57)</f>
@@ -3321,13 +3564,17 @@
       <c r="L58" s="0"/>
       <c r="M58" s="0"/>
       <c r="N58" s="0"/>
+      <c r="O58" s="5" t="n">
+        <f aca="false">D58&gt;C58</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C59" s="2" t="n">
         <f aca="false">IF(I59="Incerto",MAX(G59,J59-(ABS(F59*J59))),J59)</f>
@@ -3338,7 +3585,7 @@
         <v>0.28</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F59" s="2" t="n">
         <v>0.5</v>
@@ -3350,7 +3597,7 @@
         <v>1</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J59" s="1" t="n">
         <f aca="false">J55</f>
@@ -3362,10 +3609,14 @@
       <c r="L59" s="0"/>
       <c r="M59" s="0"/>
       <c r="N59" s="0"/>
+      <c r="O59" s="5" t="n">
+        <f aca="false">D59&gt;C59</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B60" s="0"/>
       <c r="C60" s="2" t="n">
@@ -3377,7 +3628,7 @@
         <v>0.25</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F60" s="2" t="n">
         <v>0.5</v>
@@ -3389,7 +3640,7 @@
         <v>1</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J60" s="1" t="n">
         <f aca="false">J56</f>
@@ -3399,10 +3650,14 @@
       <c r="L60" s="0"/>
       <c r="M60" s="0"/>
       <c r="N60" s="0"/>
+      <c r="O60" s="5" t="n">
+        <f aca="false">D60&gt;C60</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B61" s="0"/>
       <c r="C61" s="2" t="n">
@@ -3414,7 +3669,7 @@
         <v>0.15</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F61" s="2" t="n">
         <v>0.5</v>
@@ -3426,7 +3681,7 @@
         <v>1</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J61" s="1" t="n">
         <f aca="false">J57</f>
@@ -3436,10 +3691,14 @@
       <c r="L61" s="0"/>
       <c r="M61" s="0"/>
       <c r="N61" s="0"/>
+      <c r="O61" s="5" t="n">
+        <f aca="false">D61&gt;C61</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B62" s="0"/>
       <c r="C62" s="2" t="n">
@@ -3451,7 +3710,7 @@
         <v>0.32</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F62" s="2" t="n">
         <v>0.5</v>
@@ -3463,7 +3722,7 @@
         <v>1</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J62" s="1" t="n">
         <f aca="false">J58</f>
@@ -3473,13 +3732,17 @@
       <c r="L62" s="0"/>
       <c r="M62" s="0"/>
       <c r="N62" s="0"/>
+      <c r="O62" s="5" t="n">
+        <f aca="false">D62&gt;C62</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C63" s="2" t="n">
         <f aca="false">IF(I63="Incerto",MAX(G63,J63-(ABS(F63*J63))),J63)</f>
@@ -3490,7 +3753,7 @@
         <v>1</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F63" s="2" t="n">
         <v>3</v>
@@ -3502,7 +3765,7 @@
         <v>1</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J63" s="1" t="n">
         <v>0.5</v>
@@ -3511,13 +3774,17 @@
       <c r="L63" s="0"/>
       <c r="M63" s="0"/>
       <c r="N63" s="0"/>
+      <c r="O63" s="5" t="n">
+        <f aca="false">D63&gt;C63</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="C64" s="2" t="n">
         <f aca="false">IF(I64="Incerto",MAX(G64,J64-(ABS(F64*J64))),J64)</f>
@@ -3528,7 +3795,7 @@
         <v>1</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F64" s="2" t="n">
         <v>3</v>
@@ -3540,7 +3807,7 @@
         <v>1</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J64" s="1" t="n">
         <v>0.5</v>
@@ -3549,13 +3816,17 @@
       <c r="L64" s="0"/>
       <c r="M64" s="0"/>
       <c r="N64" s="0"/>
+      <c r="O64" s="5" t="n">
+        <f aca="false">D64&gt;C64</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C65" s="2" t="n">
         <f aca="false">IF(I65="Incerto",MAX(G65,J65-(ABS(F65*J65))),J65)</f>
@@ -3566,7 +3837,7 @@
         <v>1</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F65" s="2" t="n">
         <v>3</v>
@@ -3578,7 +3849,7 @@
         <v>1</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J65" s="1" t="n">
         <v>0.5</v>
@@ -3587,24 +3858,28 @@
       <c r="L65" s="0"/>
       <c r="M65" s="0"/>
       <c r="N65" s="0"/>
+      <c r="O65" s="5" t="n">
+        <f aca="false">D65&gt;C65</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C66" s="10" t="n">
+        <v>140</v>
+      </c>
+      <c r="C66" s="11" t="n">
         <f aca="false">IF(I66="Incerto",MAX(G66,J66-(ABS(F66*J66))),J66)</f>
         <v>0.05</v>
       </c>
-      <c r="D66" s="10" t="n">
+      <c r="D66" s="11" t="n">
         <f aca="false">IF(I66="Incerto",MIN(H66,J66+(ABS(F66*J66))),J66)</f>
-        <v>0.006</v>
+        <v>0.1</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F66" s="2" t="n">
         <v>5</v>
@@ -3617,11 +3892,11 @@
         <f aca="false">MAX(Levers_FullDesign!$D$2:$D$14)</f>
         <v>0.1</v>
       </c>
-      <c r="I66" s="5" t="s">
-        <v>30</v>
+      <c r="I66" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J66" s="1" t="n">
-        <v>0.001</v>
+        <v>0.1</v>
       </c>
       <c r="K66" s="1" t="n">
         <v>0.001</v>
@@ -3629,24 +3904,28 @@
       <c r="L66" s="0"/>
       <c r="M66" s="0"/>
       <c r="N66" s="0"/>
+      <c r="O66" s="5" t="n">
+        <f aca="false">D66&gt;C66</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C67" s="10" t="n">
+      <c r="C67" s="11" t="n">
         <f aca="false">IF(I67="Incerto",MAX(G67,J67-(ABS(F67*J67))),J67)</f>
         <v>0.05</v>
       </c>
-      <c r="D67" s="10" t="n">
+      <c r="D67" s="11" t="n">
         <f aca="false">IF(I67="Incerto",MIN(H67,J67+(ABS(F67*J67))),J67)</f>
-        <v>0.006</v>
+        <v>0.1</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F67" s="2" t="n">
         <v>5</v>
@@ -3659,11 +3938,11 @@
         <f aca="false">MAX(Levers_FullDesign!$D$2:$D$14)</f>
         <v>0.1</v>
       </c>
-      <c r="I67" s="5" t="s">
-        <v>30</v>
+      <c r="I67" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J67" s="1" t="n">
-        <v>0.001</v>
+        <v>0.1</v>
       </c>
       <c r="K67" s="1" t="n">
         <v>0.001</v>
@@ -3671,24 +3950,28 @@
       <c r="L67" s="0"/>
       <c r="M67" s="0"/>
       <c r="N67" s="0"/>
+      <c r="O67" s="5" t="n">
+        <f aca="false">D67&gt;C67</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C68" s="10" t="n">
+        <v>140</v>
+      </c>
+      <c r="C68" s="11" t="n">
         <f aca="false">IF(I68="Incerto",MAX(G68,J68-(ABS(F68*J68))),J68)</f>
         <v>0.05</v>
       </c>
-      <c r="D68" s="10" t="n">
+      <c r="D68" s="11" t="n">
         <f aca="false">IF(I68="Incerto",MIN(H68,J68+(ABS(F68*J68))),J68)</f>
-        <v>0.006</v>
+        <v>0.1</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F68" s="2" t="n">
         <v>5</v>
@@ -3701,11 +3984,11 @@
         <f aca="false">MAX(Levers_FullDesign!$D$2:$D$14)</f>
         <v>0.1</v>
       </c>
-      <c r="I68" s="5" t="s">
-        <v>30</v>
+      <c r="I68" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J68" s="1" t="n">
-        <v>0.001</v>
+        <v>0.1</v>
       </c>
       <c r="K68" s="1" t="n">
         <v>0.001</v>
@@ -3713,13 +3996,17 @@
       <c r="L68" s="0"/>
       <c r="M68" s="0"/>
       <c r="N68" s="0"/>
+      <c r="O68" s="5" t="n">
+        <f aca="false">D68&gt;C68</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C69" s="2" t="n">
         <f aca="false">IF(I69="Incerto",MAX(G69,J69-(ABS(F69*J69))),J69)</f>
@@ -3730,7 +4017,7 @@
         <v>0.375</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F69" s="2" t="n">
         <v>0.5</v>
@@ -3742,33 +4029,37 @@
       <c r="H69" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I69" s="5" t="s">
-        <v>30</v>
+      <c r="I69" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J69" s="1" t="n">
         <f aca="false">J56</f>
         <v>0.25</v>
       </c>
-      <c r="K69" s="5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L69" s="5" t="n">
+      <c r="K69" s="6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L69" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="M69" s="5" t="n">
+      <c r="M69" s="6" t="n">
         <v>1</v>
       </c>
       <c r="N69" s="1" t="n">
         <f aca="false">C69=D69</f>
         <v>0</v>
       </c>
+      <c r="O69" s="5" t="n">
+        <f aca="false">D69&gt;C69</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="C70" s="2" t="n">
         <f aca="false">IF(I70="Incerto",MAX(G70,J70-(ABS(F70*J70))),J70)</f>
@@ -3779,7 +4070,7 @@
         <v>0.225</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F70" s="2" t="n">
         <v>0.5</v>
@@ -3791,33 +4082,37 @@
       <c r="H70" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I70" s="5" t="s">
-        <v>30</v>
+      <c r="I70" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J70" s="1" t="n">
         <f aca="false">J57</f>
         <v>0.15</v>
       </c>
-      <c r="K70" s="5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L70" s="5" t="n">
+      <c r="K70" s="6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L70" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="M70" s="5" t="n">
+      <c r="M70" s="6" t="n">
         <v>1</v>
       </c>
       <c r="N70" s="1" t="n">
         <f aca="false">C70=D70</f>
         <v>0</v>
       </c>
+      <c r="O70" s="5" t="n">
+        <f aca="false">D70&gt;C70</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C71" s="2" t="n">
         <f aca="false">IF(I71="Incerto",MAX(G71,J71-(ABS(F71*J71))),J71)</f>
@@ -3828,7 +4123,7 @@
         <v>0.48</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F71" s="2" t="n">
         <v>0.5</v>
@@ -3840,33 +4135,37 @@
       <c r="H71" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I71" s="5" t="s">
-        <v>30</v>
+      <c r="I71" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J71" s="1" t="n">
         <f aca="false">J58</f>
         <v>0.32</v>
       </c>
-      <c r="K71" s="5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L71" s="5" t="n">
+      <c r="K71" s="6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L71" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="M71" s="5" t="n">
+      <c r="M71" s="6" t="n">
         <v>1</v>
       </c>
       <c r="N71" s="1" t="n">
         <f aca="false">C71=D71</f>
         <v>0</v>
       </c>
+      <c r="O71" s="5" t="n">
+        <f aca="false">D71&gt;C71</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C72" s="2" t="n">
         <f aca="false">IF(I72="Incerto",MAX(G72,J72-(ABS(F72*J72))),J72)</f>
@@ -3886,8 +4185,8 @@
       <c r="H72" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I72" s="5" t="s">
-        <v>17</v>
+      <c r="I72" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="J72" s="1" t="n">
         <v>1</v>
@@ -3901,13 +4200,17 @@
         <f aca="false">C72=D72</f>
         <v>1</v>
       </c>
+      <c r="O72" s="5" t="n">
+        <f aca="false">D72&gt;C72</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="C73" s="2" t="n">
         <f aca="false">IF(I73="Incerto",MAX(G73,J73-(ABS(F73*J73))),J73)</f>
@@ -3927,8 +4230,8 @@
       <c r="H73" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I73" s="5" t="s">
-        <v>17</v>
+      <c r="I73" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="J73" s="1" t="n">
         <v>1</v>
@@ -3942,13 +4245,17 @@
         <f aca="false">C73=D73</f>
         <v>1</v>
       </c>
+      <c r="O73" s="5" t="n">
+        <f aca="false">D73&gt;C73</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C74" s="2" t="n">
         <f aca="false">IF(I74="Incerto",MAX(G74,J74-(ABS(F74*J74))),J74)</f>
@@ -3968,8 +4275,8 @@
       <c r="H74" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I74" s="5" t="s">
-        <v>17</v>
+      <c r="I74" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="J74" s="1" t="n">
         <v>1</v>
@@ -3983,13 +4290,17 @@
         <f aca="false">C74=D74</f>
         <v>1</v>
       </c>
+      <c r="O74" s="5" t="n">
+        <f aca="false">D74&gt;C74</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C75" s="2" t="n">
         <f aca="false">IF(I75="Incerto",MAX(G75,J75-(ABS(F75*J75))),J75)</f>
@@ -4000,7 +4311,7 @@
         <v>200000</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F75" s="2" t="n">
         <v>0.5</v>
@@ -4014,7 +4325,7 @@
         <v>2000000</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J75" s="1" t="n">
         <v>200000</v>
@@ -4028,13 +4339,17 @@
         <f aca="false">C75=D75</f>
         <v>1</v>
       </c>
+      <c r="O75" s="5" t="n">
+        <f aca="false">D75&gt;C75</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="C76" s="2" t="n">
         <f aca="false">IF(I76="Incerto",MAX(G76,J76-(ABS(F76*J76))),J76)</f>
@@ -4045,7 +4360,7 @@
         <v>200000</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F76" s="2" t="n">
         <v>0.5</v>
@@ -4059,7 +4374,7 @@
         <v>2000000</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J76" s="1" t="n">
         <v>200000</v>
@@ -4073,13 +4388,17 @@
         <f aca="false">C76=D76</f>
         <v>1</v>
       </c>
+      <c r="O76" s="5" t="n">
+        <f aca="false">D76&gt;C76</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C77" s="2" t="n">
         <f aca="false">IF(I77="Incerto",MAX(G77,J77-(ABS(F77*J77))),J77)</f>
@@ -4090,7 +4409,7 @@
         <v>200000</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F77" s="2" t="n">
         <v>0.5</v>
@@ -4104,7 +4423,7 @@
         <v>2000000</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J77" s="1" t="n">
         <v>200000</v>
@@ -4118,13 +4437,17 @@
         <f aca="false">C77=D77</f>
         <v>1</v>
       </c>
+      <c r="O77" s="5" t="n">
+        <f aca="false">D77&gt;C77</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C78" s="2" t="n">
         <f aca="false">IF(I78="Incerto",MAX(G78,J78-(ABS(F78*J78))),J78)</f>
@@ -4135,7 +4458,7 @@
         <v>200000</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F78" s="2" t="n">
         <v>0.5</v>
@@ -4149,7 +4472,7 @@
         <v>2000000</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J78" s="1" t="n">
         <v>200000</v>
@@ -4163,10 +4486,15 @@
         <f aca="false">C78=D78</f>
         <v>1</v>
       </c>
+      <c r="O78" s="5" t="n">
+        <f aca="false">D78&gt;C78</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <autoFilter ref="A1:O78"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -4174,6 +4502,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4185,30 +4514,30 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4261,38 +4590,38 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.1224489795918"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="I1" s="0"/>
     </row>
@@ -4359,19 +4688,16 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
-        <v>162</v>
+      <c r="A1" s="12" t="s">
+        <v>163</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4409,149 +4735,148 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implementando mudanças para calibração
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia.xlsx
+++ b/models/dissertation-model/modelo-R/calibracao/params_calibracao_com_estrategia.xlsx
@@ -18,6 +18,10 @@
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$G$15</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">params!$A$1:$O$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">params!$A$1:$O$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">params!$A$1:$O$78</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">levers!$A$1:$H$17</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
@@ -26,6 +30,10 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">levers!$A$1:$G$15</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -869,29 +877,29 @@
   </sheetPr>
   <dimension ref="A1:O65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I81" activeCellId="0" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="43.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.9591836734694"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="2" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.56122448979592"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.85204081632653"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="6.61224489795918"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="16.3316326530612"/>
     <col collapsed="false" hidden="false" max="1023" min="16" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3874,7 +3882,7 @@
       </c>
       <c r="D66" s="10" t="n">
         <f aca="false">IF(I66="Incerto",MIN(H66,J66+(ABS(F66*J66))),J66)</f>
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>104</v>
@@ -3887,8 +3895,7 @@
         <v>0.05</v>
       </c>
       <c r="H66" s="1" t="n">
-        <f aca="false">MAX(Levers_FullDesign!$D$2:$D$14)</f>
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>31</v>
@@ -3920,7 +3927,7 @@
       </c>
       <c r="D67" s="10" t="n">
         <f aca="false">IF(I67="Incerto",MIN(H67,J67+(ABS(F67*J67))),J67)</f>
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>104</v>
@@ -3933,8 +3940,7 @@
         <v>0.05</v>
       </c>
       <c r="H67" s="1" t="n">
-        <f aca="false">MAX(Levers_FullDesign!$D$2:$D$14)</f>
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>31</v>
@@ -3966,7 +3972,7 @@
       </c>
       <c r="D68" s="10" t="n">
         <f aca="false">IF(I68="Incerto",MIN(H68,J68+(ABS(F68*J68))),J68)</f>
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>104</v>
@@ -3979,8 +3985,7 @@
         <v>0.05</v>
       </c>
       <c r="H68" s="1" t="n">
-        <f aca="false">MAX(Levers_FullDesign!$D$2:$D$14)</f>
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>31</v>
@@ -4167,24 +4172,24 @@
       </c>
       <c r="C72" s="2" t="n">
         <f aca="false">IF(I72="Incerto",MAX(G72,J72-(ABS(F72*J72))),J72)</f>
-        <v>1</v>
+        <v>0.51</v>
       </c>
       <c r="D72" s="2" t="n">
         <f aca="false">IF(I72="Incerto",MIN(H72,J72+(ABS(F72*J72))),J72)</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E72" s="0"/>
       <c r="F72" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G72" s="1" t="n">
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="H72" s="1" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="J72" s="1" t="n">
         <v>1</v>
@@ -4196,11 +4201,11 @@
       <c r="M72" s="0"/>
       <c r="N72" s="1" t="n">
         <f aca="false">C72=D72</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O72" s="1" t="n">
         <f aca="false">D72&gt;C72</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4212,24 +4217,24 @@
       </c>
       <c r="C73" s="2" t="n">
         <f aca="false">IF(I73="Incerto",MAX(G73,J73-(ABS(F73*J73))),J73)</f>
-        <v>1</v>
+        <v>0.51</v>
       </c>
       <c r="D73" s="2" t="n">
         <f aca="false">IF(I73="Incerto",MIN(H73,J73+(ABS(F73*J73))),J73)</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E73" s="0"/>
       <c r="F73" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G73" s="1" t="n">
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="H73" s="1" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="J73" s="1" t="n">
         <v>1</v>
@@ -4241,11 +4246,11 @@
       <c r="M73" s="0"/>
       <c r="N73" s="1" t="n">
         <f aca="false">C73=D73</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O73" s="1" t="n">
         <f aca="false">D73&gt;C73</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4257,24 +4262,24 @@
       </c>
       <c r="C74" s="2" t="n">
         <f aca="false">IF(I74="Incerto",MAX(G74,J74-(ABS(F74*J74))),J74)</f>
-        <v>1</v>
+        <v>0.51</v>
       </c>
       <c r="D74" s="2" t="n">
         <f aca="false">IF(I74="Incerto",MIN(H74,J74+(ABS(F74*J74))),J74)</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E74" s="0"/>
       <c r="F74" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G74" s="1" t="n">
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="H74" s="1" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="J74" s="1" t="n">
         <v>1</v>
@@ -4286,11 +4291,11 @@
       <c r="M74" s="0"/>
       <c r="N74" s="1" t="n">
         <f aca="false">C74=D74</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O74" s="1" t="n">
         <f aca="false">D74&gt;C74</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4509,19 +4514,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4554,27 +4559,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.55</v>
+        <v>0.25</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>
@@ -4602,14 +4596,14 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.44897959183673"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -4700,9 +4694,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
@@ -4750,11 +4741,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>